<commit_message>
updated Readme and japenese history
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-Japanese_1.1.2.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-Japanese_1.1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5577DAEC-66E7-41C4-B341-86A34EA7A8D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14657D57-27ED-4AEC-A6E6-358A68B90363}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="385">
   <si>
     <t>ID</t>
   </si>
@@ -3019,142 +3019,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3231,6 +3095,142 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -4550,48 +4550,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1"/>
     <row r="2" spans="2:4">
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="156" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="129"/>
+      <c r="C2" s="157"/>
+      <c r="D2" s="158"/>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="130"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="132"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="161"/>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="130"/>
-      <c r="C4" s="131"/>
-      <c r="D4" s="132"/>
+      <c r="B4" s="159"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="161"/>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="130"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="132"/>
+      <c r="B5" s="159"/>
+      <c r="C5" s="160"/>
+      <c r="D5" s="161"/>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="130"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="132"/>
+      <c r="B6" s="159"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="161"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="130"/>
-      <c r="C7" s="131"/>
-      <c r="D7" s="132"/>
+      <c r="B7" s="159"/>
+      <c r="C7" s="160"/>
+      <c r="D7" s="161"/>
     </row>
     <row r="8" spans="2:4" hidden="1">
-      <c r="B8" s="133"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="135"/>
+      <c r="B8" s="162"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="164"/>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="165" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="123"/>
-      <c r="D9" s="124"/>
+      <c r="C9" s="152"/>
+      <c r="D9" s="153"/>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="20" t="s">
@@ -4601,19 +4601,19 @@
       <c r="D10" s="22"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="121" t="s">
+      <c r="B11" s="150" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="122"/>
+      <c r="C11" s="151"/>
       <c r="D11" s="23" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="121" t="s">
+      <c r="B12" s="150" t="s">
         <v>216</v>
       </c>
-      <c r="C12" s="122"/>
+      <c r="C12" s="151"/>
       <c r="D12" s="106" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-masvs/blob/",
@@ -4623,19 +4623,19 @@
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="150" t="s">
         <v>217</v>
       </c>
-      <c r="C13" s="122"/>
+      <c r="C13" s="151"/>
       <c r="D13" s="23" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="150" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="122"/>
+      <c r="C14" s="151"/>
       <c r="D14" s="106" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
@@ -4645,69 +4645,69 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="32" customHeight="1">
-      <c r="B15" s="137" t="s">
+      <c r="B15" s="166" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="138"/>
-      <c r="D15" s="139"/>
+      <c r="C15" s="167"/>
+      <c r="D15" s="168"/>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="150" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="122"/>
+      <c r="C16" s="151"/>
       <c r="D16" s="23"/>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="145" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="126"/>
+      <c r="C17" s="155"/>
       <c r="D17" s="23"/>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="121" t="s">
+      <c r="B18" s="150" t="s">
         <v>145</v>
       </c>
-      <c r="C18" s="122"/>
+      <c r="C18" s="151"/>
       <c r="D18" s="23"/>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="150" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="122"/>
+      <c r="C19" s="151"/>
       <c r="D19" s="23"/>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="121" t="s">
+      <c r="B20" s="150" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="122"/>
+      <c r="C20" s="151"/>
       <c r="D20" s="23"/>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="121" t="s">
+      <c r="B21" s="150" t="s">
         <v>148</v>
       </c>
-      <c r="C21" s="122"/>
+      <c r="C21" s="151"/>
       <c r="D21" s="23" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="70.5" customHeight="1">
-      <c r="B22" s="121" t="s">
+      <c r="B22" s="150" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="122"/>
+      <c r="C22" s="151"/>
       <c r="D22" s="23" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="124"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="153"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="20" t="s">
@@ -4724,37 +4724,37 @@
       <c r="D25" s="23"/>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="121" t="s">
+      <c r="B26" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="122"/>
+      <c r="C26" s="151"/>
       <c r="D26" s="23"/>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="121" t="s">
+      <c r="B27" s="150" t="s">
         <v>153</v>
       </c>
-      <c r="C27" s="122"/>
+      <c r="C27" s="151"/>
       <c r="D27" s="23"/>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="121" t="s">
+      <c r="B28" s="150" t="s">
         <v>154</v>
       </c>
-      <c r="C28" s="122"/>
+      <c r="C28" s="151"/>
       <c r="D28" s="23"/>
     </row>
     <row r="29" spans="2:4" ht="52" customHeight="1">
-      <c r="B29" s="125" t="s">
+      <c r="B29" s="154" t="s">
         <v>155</v>
       </c>
-      <c r="C29" s="122"/>
+      <c r="C29" s="151"/>
       <c r="D29" s="23"/>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="123"/>
-      <c r="C30" s="123"/>
-      <c r="D30" s="124"/>
+      <c r="B30" s="152"/>
+      <c r="C30" s="152"/>
+      <c r="D30" s="153"/>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="20" t="s">
@@ -4771,37 +4771,37 @@
       <c r="D32" s="23"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="121" t="s">
+      <c r="B33" s="150" t="s">
         <v>157</v>
       </c>
-      <c r="C33" s="122"/>
+      <c r="C33" s="151"/>
       <c r="D33" s="23"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="121" t="s">
+      <c r="B34" s="150" t="s">
         <v>153</v>
       </c>
-      <c r="C34" s="122"/>
+      <c r="C34" s="151"/>
       <c r="D34" s="23"/>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="121" t="s">
+      <c r="B35" s="150" t="s">
         <v>154</v>
       </c>
-      <c r="C35" s="122"/>
+      <c r="C35" s="151"/>
       <c r="D35" s="23"/>
     </row>
     <row r="36" spans="2:4" ht="52" customHeight="1">
-      <c r="B36" s="125" t="s">
+      <c r="B36" s="154" t="s">
         <v>159</v>
       </c>
-      <c r="C36" s="122"/>
+      <c r="C36" s="151"/>
       <c r="D36" s="23"/>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="123"/>
-      <c r="C37" s="123"/>
-      <c r="D37" s="124"/>
+      <c r="B37" s="152"/>
+      <c r="C37" s="152"/>
+      <c r="D37" s="153"/>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="20" t="s">
@@ -4811,83 +4811,83 @@
       <c r="D38" s="22"/>
     </row>
     <row r="39" spans="2:4">
-      <c r="B39" s="118"/>
-      <c r="C39" s="119"/>
-      <c r="D39" s="120"/>
+      <c r="B39" s="147"/>
+      <c r="C39" s="148"/>
+      <c r="D39" s="149"/>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" s="116" t="s">
+      <c r="B40" s="145" t="s">
         <v>161</v>
       </c>
-      <c r="C40" s="117"/>
+      <c r="C40" s="146"/>
       <c r="D40" s="26"/>
     </row>
     <row r="41" spans="2:4">
-      <c r="B41" s="116" t="s">
+      <c r="B41" s="145" t="s">
         <v>162</v>
       </c>
-      <c r="C41" s="117"/>
+      <c r="C41" s="146"/>
       <c r="D41" s="26"/>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42" s="116" t="s">
+      <c r="B42" s="145" t="s">
         <v>163</v>
       </c>
-      <c r="C42" s="117"/>
+      <c r="C42" s="146"/>
       <c r="D42" s="26"/>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43" s="116" t="s">
+      <c r="B43" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="C43" s="117"/>
+      <c r="C43" s="146"/>
       <c r="D43" s="27"/>
     </row>
     <row r="44" spans="2:4">
-      <c r="B44" s="116" t="s">
+      <c r="B44" s="145" t="s">
         <v>165</v>
       </c>
-      <c r="C44" s="117"/>
+      <c r="C44" s="146"/>
       <c r="D44" s="26"/>
     </row>
     <row r="45" spans="2:4">
-      <c r="B45" s="118"/>
-      <c r="C45" s="119"/>
-      <c r="D45" s="120"/>
+      <c r="B45" s="147"/>
+      <c r="C45" s="148"/>
+      <c r="D45" s="149"/>
     </row>
     <row r="46" spans="2:4">
-      <c r="B46" s="116" t="s">
+      <c r="B46" s="145" t="s">
         <v>161</v>
       </c>
-      <c r="C46" s="117"/>
+      <c r="C46" s="146"/>
       <c r="D46" s="26"/>
     </row>
     <row r="47" spans="2:4">
-      <c r="B47" s="116" t="s">
+      <c r="B47" s="145" t="s">
         <v>162</v>
       </c>
-      <c r="C47" s="117"/>
+      <c r="C47" s="146"/>
       <c r="D47" s="26"/>
     </row>
     <row r="48" spans="2:4">
-      <c r="B48" s="116" t="s">
+      <c r="B48" s="145" t="s">
         <v>163</v>
       </c>
-      <c r="C48" s="117"/>
+      <c r="C48" s="146"/>
       <c r="D48" s="26"/>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="116" t="s">
+      <c r="B49" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="C49" s="117"/>
+      <c r="C49" s="146"/>
       <c r="D49" s="27"/>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="116" t="s">
+      <c r="B50" s="145" t="s">
         <v>165</v>
       </c>
-      <c r="C50" s="117"/>
+      <c r="C50" s="146"/>
       <c r="D50" s="26"/>
     </row>
   </sheetData>
@@ -4974,11 +4974,11 @@
       <c r="F3" s="31"/>
     </row>
     <row r="4" spans="2:24">
-      <c r="B4" s="156"/>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="156"/>
-      <c r="F4" s="156"/>
+      <c r="B4" s="173"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1">
       <c r="B5" s="32"/>
@@ -4993,16 +4993,16 @@
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
       <c r="F6" s="33"/>
-      <c r="G6" s="140" t="s">
+      <c r="G6" s="183" t="s">
         <v>167</v>
       </c>
-      <c r="H6" s="141"/>
-      <c r="I6" s="142"/>
-      <c r="V6" s="140" t="s">
+      <c r="H6" s="184"/>
+      <c r="I6" s="185"/>
+      <c r="V6" s="183" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="141"/>
-      <c r="X6" s="142"/>
+      <c r="W6" s="184"/>
+      <c r="X6" s="185"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1">
       <c r="B7" s="34"/>
@@ -5017,18 +5017,18 @@
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="143">
+      <c r="G8" s="174">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="144"/>
-      <c r="I8" s="145"/>
-      <c r="V8" s="143">
+      <c r="H8" s="175"/>
+      <c r="I8" s="176"/>
+      <c r="V8" s="174">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="144"/>
-      <c r="X8" s="145"/>
+      <c r="W8" s="175"/>
+      <c r="X8" s="176"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1">
       <c r="B9" s="33"/>
@@ -5036,12 +5036,12 @@
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
-      <c r="G9" s="146"/>
-      <c r="H9" s="147"/>
-      <c r="I9" s="148"/>
-      <c r="V9" s="146"/>
-      <c r="W9" s="147"/>
-      <c r="X9" s="148"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="178"/>
+      <c r="I9" s="179"/>
+      <c r="V9" s="177"/>
+      <c r="W9" s="178"/>
+      <c r="X9" s="179"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1">
       <c r="B10" s="34"/>
@@ -5049,12 +5049,12 @@
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
-      <c r="G10" s="146"/>
-      <c r="H10" s="147"/>
-      <c r="I10" s="148"/>
-      <c r="V10" s="146"/>
-      <c r="W10" s="147"/>
-      <c r="X10" s="148"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="178"/>
+      <c r="I10" s="179"/>
+      <c r="V10" s="177"/>
+      <c r="W10" s="178"/>
+      <c r="X10" s="179"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1">
       <c r="B11" s="34"/>
@@ -5062,19 +5062,19 @@
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
       <c r="F11" s="34"/>
-      <c r="G11" s="149"/>
-      <c r="H11" s="150"/>
-      <c r="I11" s="151"/>
-      <c r="V11" s="149"/>
-      <c r="W11" s="150"/>
-      <c r="X11" s="151"/>
+      <c r="G11" s="180"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="182"/>
+      <c r="V11" s="180"/>
+      <c r="W11" s="181"/>
+      <c r="X11" s="182"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1">
-      <c r="B12" s="152"/>
-      <c r="C12" s="152"/>
-      <c r="D12" s="152"/>
-      <c r="E12" s="152"/>
-      <c r="F12" s="152"/>
+      <c r="B12" s="169"/>
+      <c r="C12" s="169"/>
+      <c r="D12" s="169"/>
+      <c r="E12" s="169"/>
+      <c r="F12" s="169"/>
     </row>
     <row r="13" spans="2:24">
       <c r="B13" s="35"/>
@@ -5098,11 +5098,11 @@
       <c r="F15" s="34"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1">
-      <c r="B16" s="152"/>
-      <c r="C16" s="152"/>
-      <c r="D16" s="152"/>
-      <c r="E16" s="152"/>
-      <c r="F16" s="152"/>
+      <c r="B16" s="169"/>
+      <c r="C16" s="169"/>
+      <c r="D16" s="169"/>
+      <c r="E16" s="169"/>
+      <c r="F16" s="169"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="35"/>
@@ -5150,18 +5150,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1"/>
     <row r="41" spans="3:11">
-      <c r="D41" s="153" t="s">
+      <c r="D41" s="170" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="154"/>
-      <c r="F41" s="154"/>
-      <c r="G41" s="155"/>
-      <c r="H41" s="153" t="s">
+      <c r="E41" s="171"/>
+      <c r="F41" s="171"/>
+      <c r="G41" s="172"/>
+      <c r="H41" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="I41" s="154"/>
-      <c r="J41" s="154"/>
-      <c r="K41" s="155"/>
+      <c r="I41" s="171"/>
+      <c r="J41" s="171"/>
+      <c r="K41" s="172"/>
     </row>
     <row r="42" spans="3:11">
       <c r="D42" s="39" t="s">
@@ -5487,15 +5487,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G8:I11"/>
-    <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
     <mergeCell ref="H41:K41"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G8:I11"/>
+    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <phoneticPr fontId="13"/>
   <conditionalFormatting sqref="F14">
@@ -5561,23 +5561,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.5">
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="186" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="157"/>
-      <c r="I1" s="157"/>
-      <c r="J1" s="157"/>
-      <c r="K1" s="157"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="186"/>
     </row>
     <row r="2" spans="2:11">
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
     </row>
     <row r="3" spans="2:11" ht="29">
       <c r="B3" s="49" t="s">
@@ -5598,11 +5598,11 @@
       <c r="G3" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="H3" s="158" t="s">
+      <c r="H3" s="187" t="s">
         <v>184</v>
       </c>
-      <c r="I3" s="158"/>
-      <c r="J3" s="158"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
       <c r="K3" s="52" t="s">
         <v>185</v>
       </c>
@@ -5640,21 +5640,21 @@
         <v>3</v>
       </c>
       <c r="G5" s="60"/>
-      <c r="H5" s="163" t="str">
+      <c r="H5" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#architectural-information"),
 "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
-      <c r="I5" s="163" t="str">
+      <c r="I5" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05h-Testing-Platform-Interaction.md#testing-for-insecure-configuration-of-instant-apps-mstg-arch-1-mstg-arch-7"),
 "Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)")</f>
         <v>Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)</v>
       </c>
-      <c r="J5" s="175"/>
+      <c r="J5" s="129"/>
       <c r="K5" s="62"/>
     </row>
     <row r="6" spans="2:11" ht="31">
@@ -5674,21 +5674,21 @@
         <v>3</v>
       </c>
       <c r="G6" s="60"/>
-      <c r="H6" s="164" t="str">
+      <c r="H6" s="118" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),
 "Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
-      <c r="I6" s="174" t="str">
+      <c r="I6" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04h-Testing-Code-Quality.md#cross-site-scripting-flaws-mstg-arch-2-and-mstg-platform-2"),
 "Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
-      <c r="J6" s="174" t="str">
+      <c r="J6" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
@@ -5711,15 +5711,15 @@
         <v>3</v>
       </c>
       <c r="G7" s="60"/>
-      <c r="H7" s="163" t="str">
+      <c r="H7" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#architectural-information"),
 "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
-      <c r="I7" s="175"/>
-      <c r="J7" s="175"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
       <c r="K7" s="62"/>
     </row>
     <row r="8" spans="2:11">
@@ -5739,15 +5739,15 @@
         <v>3</v>
       </c>
       <c r="G8" s="60"/>
-      <c r="H8" s="163" t="str">
+      <c r="H8" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#identifying-sensitive-data"),
 "Identifying Sensitive Data")</f>
         <v>Identifying Sensitive Data</v>
       </c>
-      <c r="I8" s="175"/>
-      <c r="J8" s="175"/>
+      <c r="I8" s="129"/>
+      <c r="J8" s="129"/>
       <c r="K8" s="62"/>
     </row>
     <row r="9" spans="2:11">
@@ -5767,15 +5767,15 @@
       <c r="G9" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="163" t="str">
+      <c r="H9" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#environmental-information"),
 "Environmental Information")</f>
         <v>Environmental Information</v>
       </c>
-      <c r="I9" s="175"/>
-      <c r="J9" s="175"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="129"/>
       <c r="K9" s="62"/>
     </row>
     <row r="10" spans="2:11">
@@ -5795,15 +5795,15 @@
       <c r="G10" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="163" t="str">
+      <c r="H10" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#mapping-the-application"),
 "Mapping the Application")</f>
         <v>Mapping the Application</v>
       </c>
-      <c r="I10" s="175"/>
-      <c r="J10" s="175"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="129"/>
       <c r="K10" s="62"/>
     </row>
     <row r="11" spans="2:11">
@@ -5823,18 +5823,18 @@
       <c r="G11" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="163" t="str">
+      <c r="H11" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-for-insecure-configuration-of-instant-apps-mstg-arch-1-mstg-arch-7"),"Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)")</f>
         <v>Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)</v>
       </c>
-      <c r="I11" s="174" t="str">
+      <c r="I11" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"),
 "Principles of Testing")</f>
         <v>Principles of Testing</v>
       </c>
-      <c r="J11" s="163" t="str">
+      <c r="J11" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#penetration-testing-aka-pentesting"),
@@ -5860,15 +5860,15 @@
       <c r="G12" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="163" t="str">
+      <c r="H12" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04g-Testing-Cryptography.md#cryptographic-policy"),
 "Cryptographic policy")</f>
         <v>Cryptographic policy</v>
       </c>
-      <c r="I12" s="175"/>
-      <c r="J12" s="175"/>
+      <c r="I12" s="129"/>
+      <c r="J12" s="129"/>
       <c r="K12" s="62"/>
     </row>
     <row r="13" spans="2:11">
@@ -5888,15 +5888,15 @@
       <c r="G13" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="163" t="str">
+      <c r="H13" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"),
 "Testing enforced updating (MSTG-ARCH-9)")</f>
         <v>Testing enforced updating (MSTG-ARCH-9)</v>
       </c>
-      <c r="I13" s="175"/>
-      <c r="J13" s="175"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="129"/>
       <c r="K13" s="62"/>
     </row>
     <row r="14" spans="2:11">
@@ -5916,15 +5916,15 @@
       <c r="G14" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="163" t="str">
+      <c r="H14" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#security-testing-and-the-sdlc"),
 "Security Testing and the SDLC")</f>
         <v>Security Testing and the SDLC</v>
       </c>
-      <c r="I14" s="175"/>
-      <c r="J14" s="175"/>
+      <c r="I14" s="129"/>
+      <c r="J14" s="129"/>
       <c r="K14" s="62"/>
     </row>
     <row r="15" spans="2:11">
@@ -5938,9 +5938,9 @@
       <c r="E15" s="67"/>
       <c r="F15" s="68"/>
       <c r="G15" s="67"/>
-      <c r="H15" s="165"/>
-      <c r="I15" s="176"/>
-      <c r="J15" s="176"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
       <c r="K15" s="69"/>
     </row>
     <row r="16" spans="2:11" ht="29">
@@ -5960,15 +5960,15 @@
         <v>3</v>
       </c>
       <c r="G16" s="60"/>
-      <c r="H16" s="166" t="str">
+      <c r="H16" s="120" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
-      <c r="I16" s="168" t="str">
+      <c r="I16" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="J16" s="175"/>
+      <c r="J16" s="129"/>
       <c r="K16" s="62"/>
     </row>
     <row r="17" spans="2:11">
@@ -5984,12 +5984,12 @@
       <c r="E17" s="58"/>
       <c r="F17" s="59"/>
       <c r="G17" s="60"/>
-      <c r="H17" s="167" t="str">
+      <c r="H17" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
-      <c r="I17" s="175"/>
-      <c r="J17" s="175"/>
+      <c r="I17" s="129"/>
+      <c r="J17" s="129"/>
       <c r="K17" s="70"/>
     </row>
     <row r="18" spans="2:11">
@@ -6009,12 +6009,12 @@
         <v>3</v>
       </c>
       <c r="G18" s="60"/>
-      <c r="H18" s="168" t="str">
+      <c r="H18" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-logs-for-sensitive-data-mstg-storage-3"),"Testing Logs for Sensitive Data (MSTG-STORAGE-3)")</f>
         <v>Testing Logs for Sensitive Data (MSTG-STORAGE-3)</v>
       </c>
-      <c r="I18" s="175"/>
-      <c r="J18" s="175"/>
+      <c r="I18" s="129"/>
+      <c r="J18" s="129"/>
       <c r="K18" s="62"/>
     </row>
     <row r="19" spans="2:11">
@@ -6034,12 +6034,12 @@
         <v>3</v>
       </c>
       <c r="G19" s="60"/>
-      <c r="H19" s="167" t="str">
+      <c r="H19" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Determining Whether Sensitive Data is Sent to Third Parties (MSTG-STORAGE-4)")</f>
         <v>Determining Whether Sensitive Data is Sent to Third Parties (MSTG-STORAGE-4)</v>
       </c>
-      <c r="I19" s="175"/>
-      <c r="J19" s="175"/>
+      <c r="I19" s="129"/>
+      <c r="J19" s="129"/>
       <c r="K19" s="62"/>
     </row>
     <row r="20" spans="2:11">
@@ -6059,12 +6059,12 @@
         <v>3</v>
       </c>
       <c r="G20" s="60"/>
-      <c r="H20" s="167" t="str">
+      <c r="H20" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-the-keyboard-cache-is-disabled-for-text-input-fields-mstg-storage-5"),"Determining Whether the Keyboard Cache Is Disabled for Text Input Fields (MSTG-STORAGE-5)")</f>
         <v>Determining Whether the Keyboard Cache Is Disabled for Text Input Fields (MSTG-STORAGE-5)</v>
       </c>
-      <c r="I20" s="175"/>
-      <c r="J20" s="175"/>
+      <c r="I20" s="129"/>
+      <c r="J20" s="129"/>
       <c r="K20" s="62"/>
     </row>
     <row r="21" spans="2:11">
@@ -6084,12 +6084,12 @@
         <v>3</v>
       </c>
       <c r="G21" s="60"/>
-      <c r="H21" s="167" t="str">
+      <c r="H21" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-sensitive-stored-data-has-been-exposed-via-ipc-mechanisms-mstg-storage-6"),"Determining Whether Sensitive Stored Data Has Been Exposed via IPC Mechanisms (MSTG-STORAGE-6)")</f>
         <v>Determining Whether Sensitive Stored Data Has Been Exposed via IPC Mechanisms (MSTG-STORAGE-6)</v>
       </c>
-      <c r="I21" s="175"/>
-      <c r="J21" s="175"/>
+      <c r="I21" s="129"/>
+      <c r="J21" s="129"/>
       <c r="K21" s="62"/>
     </row>
     <row r="22" spans="2:11">
@@ -6109,12 +6109,12 @@
         <v>3</v>
       </c>
       <c r="G22" s="60"/>
-      <c r="H22" s="168" t="str">
+      <c r="H22" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosure-through-the-user-interface-mstg-storage-7"),"Checking for Sensitive Data Disclosure Through the User Interface (MSTG-STORAGE-7)")</f>
         <v>Checking for Sensitive Data Disclosure Through the User Interface (MSTG-STORAGE-7)</v>
       </c>
-      <c r="I22" s="175"/>
-      <c r="J22" s="175"/>
+      <c r="I22" s="129"/>
+      <c r="J22" s="129"/>
       <c r="K22" s="62"/>
     </row>
     <row r="23" spans="2:11">
@@ -6134,12 +6134,12 @@
       <c r="G23" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H23" s="168" t="str">
+      <c r="H23" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Testing Backups for Sensitive Data (MSTG-STORAGE-8)")</f>
         <v>Testing Backups for Sensitive Data (MSTG-STORAGE-8)</v>
       </c>
-      <c r="I23" s="175"/>
-      <c r="J23" s="175"/>
+      <c r="I23" s="129"/>
+      <c r="J23" s="129"/>
       <c r="K23" s="62"/>
     </row>
     <row r="24" spans="2:11">
@@ -6159,12 +6159,12 @@
       <c r="G24" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="168" t="str">
+      <c r="H24" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#finding-sensitive-information-in-auto-generated-screenshots-mstg-storage-9"),"Finding Sensitive Information in Auto-Generated Screenshots (MSTG-STORAGE-9)")</f>
         <v>Finding Sensitive Information in Auto-Generated Screenshots (MSTG-STORAGE-9)</v>
       </c>
-      <c r="I24" s="175"/>
-      <c r="J24" s="175"/>
+      <c r="I24" s="129"/>
+      <c r="J24" s="129"/>
       <c r="K24" s="62"/>
     </row>
     <row r="25" spans="2:11">
@@ -6184,12 +6184,12 @@
       <c r="G25" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H25" s="168" t="str">
+      <c r="H25" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#checking-memory-for-sensitive-data-mstg-storage-10"),"Checking Memory for Sensitive Data (MSTG-STORAGE-10)")</f>
         <v>Checking Memory for Sensitive Data (MSTG-STORAGE-10)</v>
       </c>
-      <c r="I25" s="175"/>
-      <c r="J25" s="175"/>
+      <c r="I25" s="129"/>
+      <c r="J25" s="129"/>
       <c r="K25" s="62"/>
     </row>
     <row r="26" spans="2:11" ht="29">
@@ -6209,15 +6209,15 @@
       <c r="G26" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H26" s="168" t="str">
+      <c r="H26" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-the-device-access-security-policy-mstg-storage-11"),"Testing the Device-Access-Security Policy (MSTG-STORAGE-11)")</f>
         <v>Testing the Device-Access-Security Policy (MSTG-STORAGE-11)</v>
       </c>
-      <c r="I26" s="174" t="str">
+      <c r="I26" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-confirm-credentials-mstg-auth-1-and-mstg-storage-11"),"Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)")</f>
         <v>Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)</v>
       </c>
-      <c r="J26" s="175"/>
+      <c r="J26" s="129"/>
       <c r="K26" s="62"/>
     </row>
     <row r="27" spans="2:11" ht="29">
@@ -6237,12 +6237,12 @@
       <c r="G27" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H27" s="169" t="str">
+      <c r="H27" s="123" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04i-Testing-user-interaction.md#testing-user-education-mstg-storage-12"),"Testing User Education (MSTG-STORAGE-12)")</f>
         <v>Testing User Education (MSTG-STORAGE-12)</v>
       </c>
-      <c r="I27" s="175"/>
-      <c r="J27" s="175"/>
+      <c r="I27" s="129"/>
+      <c r="J27" s="129"/>
       <c r="K27" s="62"/>
     </row>
     <row r="28" spans="2:11">
@@ -6256,9 +6256,9 @@
       <c r="E28" s="67"/>
       <c r="F28" s="68"/>
       <c r="G28" s="67"/>
-      <c r="H28" s="165"/>
-      <c r="I28" s="176"/>
-      <c r="J28" s="176"/>
+      <c r="H28" s="119"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="130"/>
       <c r="K28" s="69"/>
     </row>
     <row r="29" spans="2:11">
@@ -6278,15 +6278,15 @@
         <v>3</v>
       </c>
       <c r="G29" s="60"/>
-      <c r="H29" s="168" t="str">
+      <c r="H29" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="I29" s="168" t="str">
+      <c r="I29" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="J29" s="175"/>
+      <c r="J29" s="129"/>
       <c r="K29" s="62"/>
     </row>
     <row r="30" spans="2:11" ht="31">
@@ -6306,15 +6306,15 @@
         <v>3</v>
       </c>
       <c r="G30" s="60"/>
-      <c r="H30" s="168" t="str">
+      <c r="H30" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="I30" s="167" t="str">
+      <c r="I30" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
         <v>Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
       </c>
-      <c r="J30" s="175"/>
+      <c r="J30" s="129"/>
       <c r="K30" s="62"/>
     </row>
     <row r="31" spans="2:11" ht="29">
@@ -6334,15 +6334,15 @@
         <v>3</v>
       </c>
       <c r="G31" s="60"/>
-      <c r="H31" s="167" t="str">
+      <c r="H31" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
         <v>Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
       </c>
-      <c r="I31" s="168" t="str">
+      <c r="I31" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="J31" s="175"/>
+      <c r="J31" s="129"/>
       <c r="K31" s="62"/>
     </row>
     <row r="32" spans="2:11" ht="31">
@@ -6362,15 +6362,15 @@
         <v>3</v>
       </c>
       <c r="G32" s="60"/>
-      <c r="H32" s="168" t="str">
+      <c r="H32" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)")</f>
         <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)</v>
       </c>
-      <c r="I32" s="167" t="str">
+      <c r="I32" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
         <v>Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
       </c>
-      <c r="J32" s="175"/>
+      <c r="J32" s="129"/>
       <c r="K32" s="62"/>
     </row>
     <row r="33" spans="2:13">
@@ -6390,12 +6390,12 @@
         <v>3</v>
       </c>
       <c r="G33" s="60"/>
-      <c r="H33" s="168" t="str">
+      <c r="H33" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="I33" s="175"/>
-      <c r="J33" s="175"/>
+      <c r="I33" s="129"/>
+      <c r="J33" s="129"/>
       <c r="K33" s="62"/>
     </row>
     <row r="34" spans="2:13">
@@ -6415,12 +6415,12 @@
         <v>3</v>
       </c>
       <c r="G34" s="60"/>
-      <c r="H34" s="168" t="str">
+      <c r="H34" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6"),"Testing Random Number Generation (MSTG-CRYPTO-6)")</f>
         <v>Testing Random Number Generation (MSTG-CRYPTO-6)</v>
       </c>
-      <c r="I34" s="175"/>
-      <c r="J34" s="175"/>
+      <c r="I34" s="129"/>
+      <c r="J34" s="129"/>
       <c r="K34" s="62"/>
     </row>
     <row r="35" spans="2:13">
@@ -6434,9 +6434,9 @@
       <c r="E35" s="67"/>
       <c r="F35" s="68"/>
       <c r="G35" s="67"/>
-      <c r="H35" s="165"/>
-      <c r="I35" s="176"/>
-      <c r="J35" s="176"/>
+      <c r="H35" s="119"/>
+      <c r="I35" s="130"/>
+      <c r="J35" s="130"/>
       <c r="K35" s="69"/>
     </row>
     <row r="36" spans="2:13" ht="29">
@@ -6456,15 +6456,15 @@
         <v>3</v>
       </c>
       <c r="G36" s="60"/>
-      <c r="H36" s="168" t="str">
+      <c r="H36" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-confirm-credentials-mstg-auth-1-and-mstg-storage-11"),"Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)")</f>
         <v>Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)</v>
       </c>
-      <c r="I36" s="174" t="str">
+      <c r="I36" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
-      <c r="J36" s="174" t="str">
+      <c r="J36" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
@@ -6487,12 +6487,12 @@
         <v>3</v>
       </c>
       <c r="G37" s="60"/>
-      <c r="H37" s="168" t="str">
+      <c r="H37" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Testing Stateful Session Management (MSTG-AUTH-2)")</f>
         <v>Testing Stateful Session Management (MSTG-AUTH-2)</v>
       </c>
-      <c r="I37" s="175"/>
-      <c r="J37" s="175"/>
+      <c r="I37" s="129"/>
+      <c r="J37" s="129"/>
       <c r="K37" s="62"/>
     </row>
     <row r="38" spans="2:13" ht="29">
@@ -6512,15 +6512,15 @@
         <v>3</v>
       </c>
       <c r="G38" s="60"/>
-      <c r="H38" s="167" t="str">
+      <c r="H38" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)")</f>
         <v>Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)</v>
       </c>
-      <c r="I38" s="174" t="str">
+      <c r="I38" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J38" s="175"/>
+      <c r="J38" s="129"/>
       <c r="K38" s="62"/>
       <c r="M38" s="73"/>
     </row>
@@ -6537,12 +6537,12 @@
       <c r="E39" s="58"/>
       <c r="F39" s="59"/>
       <c r="G39" s="60"/>
-      <c r="H39" s="168" t="str">
+      <c r="H39" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Testing User Logout (MSTG-AUTH-4)")</f>
         <v>Testing User Logout (MSTG-AUTH-4)</v>
       </c>
-      <c r="I39" s="175"/>
-      <c r="J39" s="175"/>
+      <c r="I39" s="129"/>
+      <c r="J39" s="129"/>
       <c r="K39" s="62"/>
       <c r="M39" s="73"/>
     </row>
@@ -6563,12 +6563,12 @@
         <v>3</v>
       </c>
       <c r="G40" s="60"/>
-      <c r="H40" s="168" t="str">
+      <c r="H40" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
-      <c r="I40" s="175"/>
-      <c r="J40" s="175"/>
+      <c r="I40" s="129"/>
+      <c r="J40" s="129"/>
       <c r="K40" s="62"/>
     </row>
     <row r="41" spans="2:13">
@@ -6588,15 +6588,15 @@
         <v>3</v>
       </c>
       <c r="G41" s="60"/>
-      <c r="H41" s="168" t="str">
+      <c r="H41" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
-      <c r="I41" s="174" t="str">
+      <c r="I41" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
         <v>Dynamic Testing (MSTG-AUTH-6)</v>
       </c>
-      <c r="J41" s="175"/>
+      <c r="J41" s="129"/>
       <c r="K41" s="62"/>
     </row>
     <row r="42" spans="2:13" ht="29">
@@ -6616,12 +6616,12 @@
         <v>3</v>
       </c>
       <c r="G42" s="60"/>
-      <c r="H42" s="168" t="str">
+      <c r="H42" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Testing Session Timeout (MSTG-AUTH-7)")</f>
         <v>Testing Session Timeout (MSTG-AUTH-7)</v>
       </c>
-      <c r="I42" s="177"/>
-      <c r="J42" s="177"/>
+      <c r="I42" s="131"/>
+      <c r="J42" s="131"/>
       <c r="K42" s="74"/>
     </row>
     <row r="43" spans="2:13" ht="29">
@@ -6641,12 +6641,12 @@
       <c r="G43" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H43" s="168" t="str">
+      <c r="H43" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-biometric-authentication-mstg-auth-8"),"Testing Biometric Authentication (MSTG-AUTH-8)")</f>
         <v>Testing Biometric Authentication (MSTG-AUTH-8)</v>
       </c>
-      <c r="I43" s="175"/>
-      <c r="J43" s="175"/>
+      <c r="I43" s="129"/>
+      <c r="J43" s="129"/>
       <c r="K43" s="62"/>
     </row>
     <row r="44" spans="2:13" ht="29">
@@ -6666,12 +6666,12 @@
       <c r="G44" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H44" s="168" t="str">
+      <c r="H44" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
-      <c r="I44" s="175"/>
-      <c r="J44" s="175"/>
+      <c r="I44" s="129"/>
+      <c r="J44" s="129"/>
       <c r="K44" s="62"/>
     </row>
     <row r="45" spans="2:13">
@@ -6691,12 +6691,12 @@
       <c r="G45" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H45" s="168" t="str">
+      <c r="H45" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
-      <c r="I45" s="175"/>
-      <c r="J45" s="175"/>
+      <c r="I45" s="129"/>
+      <c r="J45" s="129"/>
       <c r="K45" s="62"/>
     </row>
     <row r="46" spans="2:13" ht="29">
@@ -6716,12 +6716,12 @@
       <c r="G46" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H46" s="170" t="str">
+      <c r="H46" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"),"Testing Login Activity and Device Blocking (MSTG-AUTH-11)")</f>
         <v>Testing Login Activity and Device Blocking (MSTG-AUTH-11)</v>
       </c>
-      <c r="I46" s="175"/>
-      <c r="J46" s="175"/>
+      <c r="I46" s="129"/>
+      <c r="J46" s="129"/>
       <c r="K46" s="62"/>
     </row>
     <row r="47" spans="2:13">
@@ -6735,9 +6735,9 @@
       <c r="E47" s="67"/>
       <c r="F47" s="68"/>
       <c r="G47" s="67"/>
-      <c r="H47" s="165"/>
-      <c r="I47" s="176"/>
-      <c r="J47" s="176"/>
+      <c r="H47" s="119"/>
+      <c r="I47" s="130"/>
+      <c r="J47" s="130"/>
       <c r="K47" s="69"/>
     </row>
     <row r="48" spans="2:13" ht="29">
@@ -6757,12 +6757,12 @@
         <v>3</v>
       </c>
       <c r="G48" s="60"/>
-      <c r="H48" s="168" t="str">
+      <c r="H48" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
-      <c r="I48" s="175"/>
-      <c r="J48" s="175"/>
+      <c r="I48" s="129"/>
+      <c r="J48" s="129"/>
       <c r="K48" s="62"/>
     </row>
     <row r="49" spans="2:11" ht="43.5">
@@ -6782,12 +6782,12 @@
         <v>3</v>
       </c>
       <c r="G49" s="60"/>
-      <c r="H49" s="168" t="str">
+      <c r="H49" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
-      <c r="I49" s="175"/>
-      <c r="J49" s="175"/>
+      <c r="I49" s="129"/>
+      <c r="J49" s="129"/>
       <c r="K49" s="62"/>
     </row>
     <row r="50" spans="2:11" ht="29">
@@ -6807,12 +6807,12 @@
         <v>3</v>
       </c>
       <c r="G50" s="60"/>
-      <c r="H50" s="168" t="str">
+      <c r="H50" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-endpoint-identify-verification-mstg-network-3"),"Testing Endpoint Identify Verification (MSTG-NETWORK-3)")</f>
         <v>Testing Endpoint Identify Verification (MSTG-NETWORK-3)</v>
       </c>
-      <c r="I50" s="174"/>
-      <c r="J50" s="174"/>
+      <c r="I50" s="128"/>
+      <c r="J50" s="128"/>
       <c r="K50" s="75"/>
     </row>
     <row r="51" spans="2:11" ht="29">
@@ -6832,15 +6832,15 @@
       <c r="G51" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H51" s="168" t="str">
+      <c r="H51" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-4)</v>
       </c>
-      <c r="I51" s="168" t="str">
+      <c r="I51" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-network-security-configuration-settings-mstg-network-4"),"Testing the Network Security Configuration settings (MSTG-NETWORK-4)")</f>
         <v>Testing the Network Security Configuration settings (MSTG-NETWORK-4)</v>
       </c>
-      <c r="J51" s="175"/>
+      <c r="J51" s="129"/>
       <c r="K51" s="62"/>
     </row>
     <row r="52" spans="2:11" ht="29">
@@ -6860,12 +6860,12 @@
       <c r="G52" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H52" s="168" t="str">
+      <c r="H52" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
         <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
       </c>
-      <c r="I52" s="175"/>
-      <c r="J52" s="175"/>
+      <c r="I52" s="129"/>
+      <c r="J52" s="129"/>
       <c r="K52" s="62"/>
     </row>
     <row r="53" spans="2:11">
@@ -6885,12 +6885,12 @@
       <c r="G53" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H53" s="168" t="str">
+      <c r="H53" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-security-provider-mstg-network-6"),"Testing the Security Provider (MSTG-NETWORK-6)")</f>
         <v>Testing the Security Provider (MSTG-NETWORK-6)</v>
       </c>
-      <c r="I53" s="175"/>
-      <c r="J53" s="175"/>
+      <c r="I53" s="129"/>
+      <c r="J53" s="129"/>
       <c r="K53" s="62"/>
     </row>
     <row r="54" spans="2:11">
@@ -6904,9 +6904,9 @@
       <c r="E54" s="67"/>
       <c r="F54" s="68"/>
       <c r="G54" s="67"/>
-      <c r="H54" s="165"/>
-      <c r="I54" s="176"/>
-      <c r="J54" s="176"/>
+      <c r="H54" s="119"/>
+      <c r="I54" s="130"/>
+      <c r="J54" s="130"/>
       <c r="K54" s="69"/>
     </row>
     <row r="55" spans="2:11">
@@ -6926,12 +6926,12 @@
         <v>3</v>
       </c>
       <c r="G55" s="60"/>
-      <c r="H55" s="168" t="str">
+      <c r="H55" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Testing App Permissions (MSTG-PLATFORM-1)")</f>
         <v>Testing App Permissions (MSTG-PLATFORM-1)</v>
       </c>
-      <c r="I55" s="175"/>
-      <c r="J55" s="175"/>
+      <c r="I55" s="129"/>
+      <c r="J55" s="129"/>
       <c r="K55" s="62"/>
     </row>
     <row r="56" spans="2:11" ht="29">
@@ -6951,15 +6951,15 @@
         <v>3</v>
       </c>
       <c r="G56" s="60"/>
-      <c r="H56" s="168" t="str">
+      <c r="H56" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#testing-for-injection-flaws-mstg-platform-2"),"Testing for Injection Flaws (MSTG-PLATFORM-2)")</f>
         <v>Testing for Injection Flaws (MSTG-PLATFORM-2)</v>
       </c>
-      <c r="I56" s="168" t="str">
+      <c r="I56" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#testing-for-fragment-injection-mstg-platform-2"),"Testing for Fragment Injection (MSTG-PLATFORM-2)")</f>
         <v>Testing for Fragment Injection (MSTG-PLATFORM-2)</v>
       </c>
-      <c r="J56" s="175"/>
+      <c r="J56" s="129"/>
       <c r="K56" s="62"/>
     </row>
     <row r="57" spans="2:11" ht="29">
@@ -6979,12 +6979,12 @@
         <v>3</v>
       </c>
       <c r="G57" s="60"/>
-      <c r="H57" s="168" t="str">
+      <c r="H57" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Testing Custom URL Schemes (MSTG-PLATFORM-3)")</f>
         <v>Testing Custom URL Schemes (MSTG-PLATFORM-3)</v>
       </c>
-      <c r="I57" s="175"/>
-      <c r="J57" s="175"/>
+      <c r="I57" s="129"/>
+      <c r="J57" s="129"/>
       <c r="K57" s="62"/>
     </row>
     <row r="58" spans="2:11">
@@ -7004,12 +7004,12 @@
         <v>3</v>
       </c>
       <c r="G58" s="60"/>
-      <c r="H58" s="168" t="str">
+      <c r="H58" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"),"Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)")</f>
         <v>Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)</v>
       </c>
-      <c r="I58" s="175"/>
-      <c r="J58" s="175"/>
+      <c r="I58" s="129"/>
+      <c r="J58" s="129"/>
       <c r="K58" s="62"/>
     </row>
     <row r="59" spans="2:11">
@@ -7029,12 +7029,12 @@
         <v>3</v>
       </c>
       <c r="G59" s="60"/>
-      <c r="H59" s="168" t="str">
+      <c r="H59" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-javascript-execution-in-webviews-mstg-platform-5"),"Testing JavaScript Execution in WebViews (MSTG-PLATFORM-5)")</f>
         <v>Testing JavaScript Execution in WebViews (MSTG-PLATFORM-5)</v>
       </c>
-      <c r="I59" s="175"/>
-      <c r="J59" s="175"/>
+      <c r="I59" s="129"/>
+      <c r="J59" s="129"/>
       <c r="K59" s="62"/>
     </row>
     <row r="60" spans="2:11" ht="29">
@@ -7054,12 +7054,12 @@
         <v>3</v>
       </c>
       <c r="G60" s="60"/>
-      <c r="H60" s="168" t="str">
+      <c r="H60" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Testing WebView Protocol Handlers (MSTG-PLATFORM-6)")</f>
         <v>Testing WebView Protocol Handlers (MSTG-PLATFORM-6)</v>
       </c>
-      <c r="I60" s="175"/>
-      <c r="J60" s="175"/>
+      <c r="I60" s="129"/>
+      <c r="J60" s="129"/>
       <c r="K60" s="62"/>
     </row>
     <row r="61" spans="2:11" ht="29">
@@ -7079,12 +7079,12 @@
         <v>3</v>
       </c>
       <c r="G61" s="60"/>
-      <c r="H61" s="168" t="str">
+      <c r="H61" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#determining-whether-java-objects-are-exposed-through-webviews-mstg-platform-7"),"Determining Whether Java Objects Are Exposed Through WebViews (MSTG-PLATFORM-7)")</f>
         <v>Determining Whether Java Objects Are Exposed Through WebViews (MSTG-PLATFORM-7)</v>
       </c>
-      <c r="I61" s="175"/>
-      <c r="J61" s="175"/>
+      <c r="I61" s="129"/>
+      <c r="J61" s="129"/>
       <c r="K61" s="62"/>
     </row>
     <row r="62" spans="2:11" ht="29">
@@ -7104,12 +7104,12 @@
         <v>3</v>
       </c>
       <c r="G62" s="60"/>
-      <c r="H62" s="168" t="str">
+      <c r="H62" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Testing Object Persistence (MSTG-PLATFORM-8)")</f>
         <v>Testing Object Persistence (MSTG-PLATFORM-8)</v>
       </c>
-      <c r="I62" s="175"/>
-      <c r="J62" s="175"/>
+      <c r="I62" s="129"/>
+      <c r="J62" s="129"/>
       <c r="K62" s="62"/>
     </row>
     <row r="63" spans="2:11">
@@ -7123,9 +7123,9 @@
       <c r="E63" s="67"/>
       <c r="F63" s="68"/>
       <c r="G63" s="67"/>
-      <c r="H63" s="165"/>
-      <c r="I63" s="176"/>
-      <c r="J63" s="176"/>
+      <c r="H63" s="119"/>
+      <c r="I63" s="130"/>
+      <c r="J63" s="130"/>
       <c r="K63" s="69"/>
     </row>
     <row r="64" spans="2:11">
@@ -7145,12 +7145,12 @@
         <v>3</v>
       </c>
       <c r="G64" s="60"/>
-      <c r="H64" s="168" t="str">
+      <c r="H64" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Making Sure That the App is Properly Signed (MSTG-CODE-1)")</f>
         <v>Making Sure That the App is Properly Signed (MSTG-CODE-1)</v>
       </c>
-      <c r="I64" s="175"/>
-      <c r="J64" s="175"/>
+      <c r="I64" s="129"/>
+      <c r="J64" s="129"/>
       <c r="K64" s="62"/>
     </row>
     <row r="65" spans="2:12">
@@ -7170,12 +7170,12 @@
         <v>3</v>
       </c>
       <c r="G65" s="60"/>
-      <c r="H65" s="168" t="str">
+      <c r="H65" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-whether-the-app-is-debuggable-mstg-code-2"),"Testing Whether the App is Debuggable (MSTG-CODE-2)")</f>
         <v>Testing Whether the App is Debuggable (MSTG-CODE-2)</v>
       </c>
-      <c r="I65" s="175"/>
-      <c r="J65" s="175"/>
+      <c r="I65" s="129"/>
+      <c r="J65" s="129"/>
       <c r="K65" s="62"/>
     </row>
     <row r="66" spans="2:12">
@@ -7195,12 +7195,12 @@
         <v>3</v>
       </c>
       <c r="G66" s="60"/>
-      <c r="H66" s="168" t="str">
+      <c r="H66" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-for-debugging-symbols-mstg-code-3"),"Testing for Debugging Symbols (MSTG-CODE-3)")</f>
         <v>Testing for Debugging Symbols (MSTG-CODE-3)</v>
       </c>
-      <c r="I66" s="175"/>
-      <c r="J66" s="175"/>
+      <c r="I66" s="129"/>
+      <c r="J66" s="129"/>
       <c r="K66" s="62"/>
     </row>
     <row r="67" spans="2:12">
@@ -7220,12 +7220,12 @@
         <v>3</v>
       </c>
       <c r="G67" s="60"/>
-      <c r="H67" s="168" t="str">
+      <c r="H67" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-for-debugging-code-and-verbose-error-logging-mstg-code-4"),"Testing for Debugging Code and Verbose Error Logging (MSTG-CODE-4)")</f>
         <v>Testing for Debugging Code and Verbose Error Logging (MSTG-CODE-4)</v>
       </c>
-      <c r="I67" s="175"/>
-      <c r="J67" s="175"/>
+      <c r="I67" s="129"/>
+      <c r="J67" s="129"/>
       <c r="K67" s="62"/>
     </row>
     <row r="68" spans="2:12" ht="29">
@@ -7245,12 +7245,12 @@
         <v>3</v>
       </c>
       <c r="G68" s="60"/>
-      <c r="H68" s="170" t="str">
+      <c r="H68" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
-      <c r="I68" s="175"/>
-      <c r="J68" s="175"/>
+      <c r="I68" s="129"/>
+      <c r="J68" s="129"/>
       <c r="K68" s="62"/>
     </row>
     <row r="69" spans="2:12">
@@ -7270,12 +7270,12 @@
         <v>3</v>
       </c>
       <c r="G69" s="60"/>
-      <c r="H69" s="168" t="str">
+      <c r="H69" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6-and-mstg-code-7"),"Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)</v>
       </c>
-      <c r="I69" s="175"/>
-      <c r="J69" s="175"/>
+      <c r="I69" s="129"/>
+      <c r="J69" s="129"/>
       <c r="K69" s="62"/>
     </row>
     <row r="70" spans="2:12">
@@ -7295,12 +7295,12 @@
         <v>3</v>
       </c>
       <c r="G70" s="60"/>
-      <c r="H70" s="168" t="str">
+      <c r="H70" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6-and-mstg-code-7"),"Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)</v>
       </c>
-      <c r="I70" s="175"/>
-      <c r="J70" s="175"/>
+      <c r="I70" s="129"/>
+      <c r="J70" s="129"/>
       <c r="K70" s="62"/>
     </row>
     <row r="71" spans="2:12">
@@ -7320,12 +7320,12 @@
         <v>3</v>
       </c>
       <c r="G71" s="60"/>
-      <c r="H71" s="168" t="str">
+      <c r="H71" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#memory-corruption-bugs-mstg-code-8"),"Memory Corruption Bugs (MSTG-CODE-8)")</f>
         <v>Memory Corruption Bugs (MSTG-CODE-8)</v>
       </c>
-      <c r="I71" s="175"/>
-      <c r="J71" s="175"/>
+      <c r="I71" s="129"/>
+      <c r="J71" s="129"/>
       <c r="K71" s="76"/>
       <c r="L71" s="77"/>
     </row>
@@ -7346,12 +7346,12 @@
         <v>3</v>
       </c>
       <c r="G72" s="60"/>
-      <c r="H72" s="168" t="str">
+      <c r="H72" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Make Sure That Free Security Features Are Activated (MSTG-CODE-9)")</f>
         <v>Make Sure That Free Security Features Are Activated (MSTG-CODE-9)</v>
       </c>
-      <c r="I72" s="175"/>
-      <c r="J72" s="175"/>
+      <c r="I72" s="129"/>
+      <c r="J72" s="129"/>
       <c r="K72" s="62"/>
     </row>
     <row r="73" spans="2:12">
@@ -7361,9 +7361,9 @@
       <c r="E73" s="80"/>
       <c r="F73" s="80"/>
       <c r="G73" s="80"/>
-      <c r="H73" s="171"/>
-      <c r="I73" s="178"/>
-      <c r="J73" s="178"/>
+      <c r="H73" s="125"/>
+      <c r="I73" s="132"/>
+      <c r="J73" s="132"/>
       <c r="K73" s="81"/>
     </row>
     <row r="74" spans="2:12">
@@ -7373,9 +7373,9 @@
       <c r="E74" s="38"/>
       <c r="F74" s="38"/>
       <c r="G74" s="38"/>
-      <c r="H74" s="172"/>
-      <c r="I74" s="172"/>
-      <c r="J74" s="172"/>
+      <c r="H74" s="126"/>
+      <c r="I74" s="126"/>
+      <c r="J74" s="126"/>
       <c r="K74" s="61"/>
     </row>
     <row r="75" spans="2:12">
@@ -7385,9 +7385,9 @@
       <c r="E75" s="38"/>
       <c r="F75" s="38"/>
       <c r="G75" s="38"/>
-      <c r="H75" s="172"/>
-      <c r="I75" s="172"/>
-      <c r="J75" s="172"/>
+      <c r="H75" s="126"/>
+      <c r="I75" s="126"/>
+      <c r="J75" s="126"/>
       <c r="K75" s="61"/>
     </row>
     <row r="76" spans="2:12">
@@ -7397,9 +7397,9 @@
       <c r="E76" s="38"/>
       <c r="F76" s="38"/>
       <c r="G76" s="38"/>
-      <c r="H76" s="172"/>
-      <c r="I76" s="172"/>
-      <c r="J76" s="172"/>
+      <c r="H76" s="126"/>
+      <c r="I76" s="126"/>
+      <c r="J76" s="126"/>
       <c r="K76" s="61"/>
     </row>
     <row r="77" spans="2:12">
@@ -7411,9 +7411,9 @@
       <c r="E77" s="38"/>
       <c r="F77" s="38"/>
       <c r="G77" s="38"/>
-      <c r="H77" s="172"/>
-      <c r="I77" s="172"/>
-      <c r="J77" s="172"/>
+      <c r="H77" s="126"/>
+      <c r="I77" s="126"/>
+      <c r="J77" s="126"/>
       <c r="K77" s="61"/>
     </row>
     <row r="78" spans="2:12" ht="29">
@@ -7427,9 +7427,9 @@
       <c r="E78" s="38"/>
       <c r="F78" s="38"/>
       <c r="G78" s="38"/>
-      <c r="H78" s="172"/>
-      <c r="I78" s="172"/>
-      <c r="J78" s="172"/>
+      <c r="H78" s="126"/>
+      <c r="I78" s="126"/>
+      <c r="J78" s="126"/>
       <c r="K78" s="61"/>
     </row>
     <row r="79" spans="2:12">
@@ -7443,9 +7443,9 @@
       <c r="E79" s="38"/>
       <c r="F79" s="38"/>
       <c r="G79" s="38"/>
-      <c r="H79" s="172"/>
-      <c r="I79" s="172"/>
-      <c r="J79" s="172"/>
+      <c r="H79" s="126"/>
+      <c r="I79" s="126"/>
+      <c r="J79" s="126"/>
       <c r="K79" s="61"/>
     </row>
     <row r="80" spans="2:12">
@@ -7459,9 +7459,9 @@
       <c r="E80" s="38"/>
       <c r="F80" s="38"/>
       <c r="G80" s="38"/>
-      <c r="H80" s="172"/>
-      <c r="I80" s="172"/>
-      <c r="J80" s="172"/>
+      <c r="H80" s="126"/>
+      <c r="I80" s="126"/>
+      <c r="J80" s="126"/>
       <c r="K80" s="61"/>
     </row>
     <row r="81" spans="2:11">
@@ -7475,9 +7475,9 @@
       <c r="E81" s="38"/>
       <c r="F81" s="38"/>
       <c r="G81" s="38"/>
-      <c r="H81" s="172"/>
-      <c r="I81" s="172"/>
-      <c r="J81" s="172"/>
+      <c r="H81" s="126"/>
+      <c r="I81" s="126"/>
+      <c r="J81" s="126"/>
       <c r="K81" s="61"/>
     </row>
     <row r="82" spans="2:11">
@@ -7487,9 +7487,9 @@
       <c r="E82" s="38"/>
       <c r="F82" s="38"/>
       <c r="G82" s="38"/>
-      <c r="H82" s="172"/>
-      <c r="I82" s="173"/>
-      <c r="J82" s="173"/>
+      <c r="H82" s="126"/>
+      <c r="I82" s="127"/>
+      <c r="J82" s="127"/>
       <c r="K82" s="61"/>
     </row>
     <row r="83" spans="2:11">
@@ -7499,9 +7499,9 @@
       <c r="E83" s="38"/>
       <c r="F83" s="38"/>
       <c r="G83" s="38"/>
-      <c r="H83" s="172"/>
-      <c r="I83" s="173"/>
-      <c r="J83" s="173"/>
+      <c r="H83" s="126"/>
+      <c r="I83" s="127"/>
+      <c r="J83" s="127"/>
       <c r="K83" s="61"/>
     </row>
     <row r="84" spans="2:11">
@@ -7511,9 +7511,9 @@
       <c r="E84" s="38"/>
       <c r="F84" s="38"/>
       <c r="G84" s="38"/>
-      <c r="H84" s="172"/>
-      <c r="I84" s="173"/>
-      <c r="J84" s="173"/>
+      <c r="H84" s="126"/>
+      <c r="I84" s="127"/>
+      <c r="J84" s="127"/>
       <c r="K84" s="61"/>
     </row>
     <row r="85" spans="2:11">
@@ -7523,9 +7523,9 @@
       <c r="E85" s="38"/>
       <c r="F85" s="38"/>
       <c r="G85" s="38"/>
-      <c r="H85" s="173"/>
-      <c r="I85" s="173"/>
-      <c r="J85" s="173"/>
+      <c r="H85" s="127"/>
+      <c r="I85" s="127"/>
+      <c r="J85" s="127"/>
       <c r="K85" s="61"/>
     </row>
   </sheetData>
@@ -7582,7 +7582,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="38"/>
       <c r="F1" s="38"/>
-      <c r="G1" s="173"/>
+      <c r="G1" s="127"/>
       <c r="H1" s="61"/>
     </row>
     <row r="2" spans="2:8">
@@ -7591,7 +7591,7 @@
       <c r="D2" s="61"/>
       <c r="E2" s="38"/>
       <c r="F2" s="38"/>
-      <c r="G2" s="173"/>
+      <c r="G2" s="127"/>
       <c r="H2" s="61"/>
     </row>
     <row r="3" spans="2:8">
@@ -7610,7 +7610,7 @@
       <c r="F3" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="G3" s="179" t="s">
+      <c r="G3" s="133" t="s">
         <v>383</v>
       </c>
       <c r="H3" s="52" t="s">
@@ -7627,7 +7627,7 @@
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="67"/>
-      <c r="G4" s="180"/>
+      <c r="G4" s="134"/>
       <c r="H4" s="69"/>
     </row>
     <row r="5" spans="2:8" ht="29">
@@ -7646,7 +7646,7 @@
       <c r="F5" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="181" t="str">
+      <c r="G5" s="135" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-root-detection-mstg-resilience-1"),"Testing Root Detection (MSTG-RESILIENCE-1)")</f>
         <v>Testing Root Detection (MSTG-RESILIENCE-1)</v>
       </c>
@@ -7668,7 +7668,7 @@
       <c r="F6" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="182" t="str">
+      <c r="G6" s="136" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-anti-debugging-detection-mstg-resilience-2"),"Testing Anti-Debugging Detection (MSTG-RESILIENCE-2)")</f>
         <v>Testing Anti-Debugging Detection (MSTG-RESILIENCE-2)</v>
       </c>
@@ -7690,7 +7690,7 @@
       <c r="F7" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="181" t="str">
+      <c r="G7" s="135" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-file-integrity-checks-mstg-resilience-3"),"Testing File Integrity Checks (MSTG-RESILIENCE-3)")</f>
         <v>Testing File Integrity Checks (MSTG-RESILIENCE-3)</v>
       </c>
@@ -7712,7 +7712,7 @@
       <c r="F8" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="168" t="str">
+      <c r="G8" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-reverse-engineering-tools-detection-mstg-resilience-4"),"Testing Reverse Engineering Tools Detection (MSTG-RESILIENCE-4)")</f>
         <v>Testing Reverse Engineering Tools Detection (MSTG-RESILIENCE-4)</v>
       </c>
@@ -7734,7 +7734,7 @@
       <c r="F9" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="181" t="str">
+      <c r="G9" s="135" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-emulator-detection-mstg-resilience-5"),"Testing Emulator Detection (MSTG-RESILIENCE-5)")</f>
         <v>Testing Emulator Detection (MSTG-RESILIENCE-5)</v>
       </c>
@@ -7756,7 +7756,7 @@
       <c r="F10" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="168" t="str">
+      <c r="G10" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-run-time-integrity-checks-mstg-resilience-6"),"Testing Run Time Integrity Checks (MSTG-RESILIENCE-6)")</f>
         <v>Testing Run Time Integrity Checks (MSTG-RESILIENCE-6)</v>
       </c>
@@ -7778,7 +7778,7 @@
       <c r="F11" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="183" t="s">
+      <c r="G11" s="137" t="s">
         <v>384</v>
       </c>
       <c r="H11" s="62"/>
@@ -7799,7 +7799,7 @@
       <c r="F12" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="184" t="s">
+      <c r="G12" s="138" t="s">
         <v>79</v>
       </c>
       <c r="H12" s="62"/>
@@ -7820,7 +7820,7 @@
       <c r="F13" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="168" t="str">
+      <c r="G13" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation-mstg-resilience-9"),"Testing Obfuscation (MSTG-RESILIENCE-9)")</f>
         <v>Testing Obfuscation (MSTG-RESILIENCE-9)</v>
       </c>
@@ -7834,7 +7834,7 @@
       </c>
       <c r="E14" s="67"/>
       <c r="F14" s="67"/>
-      <c r="G14" s="180"/>
+      <c r="G14" s="134"/>
       <c r="H14" s="69"/>
     </row>
     <row r="15" spans="2:8" ht="29">
@@ -7853,7 +7853,7 @@
       <c r="F15" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="168" t="str">
+      <c r="G15" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-device-binding-mstg-resilience-10"),"Testing Device Binding (MSTG-RESILIENCE-10)")</f>
         <v>Testing Device Binding (MSTG-RESILIENCE-10)</v>
       </c>
@@ -7867,7 +7867,7 @@
       </c>
       <c r="E16" s="67"/>
       <c r="F16" s="67"/>
-      <c r="G16" s="180"/>
+      <c r="G16" s="134"/>
       <c r="H16" s="69"/>
     </row>
     <row r="17" spans="2:8" ht="43.5">
@@ -7886,7 +7886,7 @@
       <c r="F17" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="168" t="str">
+      <c r="G17" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation-mstg-resilience-9"),"Testing Obfuscation (MSTG-RESILIENCE-9)")</f>
         <v>Testing Obfuscation (MSTG-RESILIENCE-9)</v>
       </c>
@@ -7908,7 +7908,7 @@
       <c r="F18" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="184" t="s">
+      <c r="G18" s="138" t="s">
         <v>384</v>
       </c>
       <c r="H18" s="62"/>
@@ -7919,7 +7919,7 @@
       <c r="D19" s="79"/>
       <c r="E19" s="80"/>
       <c r="F19" s="80"/>
-      <c r="G19" s="185"/>
+      <c r="G19" s="139"/>
       <c r="H19" s="81"/>
     </row>
     <row r="20" spans="2:8">
@@ -7928,7 +7928,7 @@
       <c r="D20" s="61"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
-      <c r="G20" s="172"/>
+      <c r="G20" s="126"/>
       <c r="H20" s="61"/>
     </row>
     <row r="21" spans="2:8">
@@ -7937,7 +7937,7 @@
       <c r="D21" s="61"/>
       <c r="E21" s="38"/>
       <c r="F21" s="38"/>
-      <c r="G21" s="172"/>
+      <c r="G21" s="126"/>
       <c r="H21" s="61"/>
     </row>
     <row r="22" spans="2:8">
@@ -7948,7 +7948,7 @@
       <c r="D22" s="61"/>
       <c r="E22" s="38"/>
       <c r="F22" s="38"/>
-      <c r="G22" s="172"/>
+      <c r="G22" s="126"/>
       <c r="H22" s="61"/>
     </row>
     <row r="23" spans="2:8" ht="29">
@@ -7961,7 +7961,7 @@
       </c>
       <c r="E23" s="38"/>
       <c r="F23" s="38"/>
-      <c r="G23" s="172"/>
+      <c r="G23" s="126"/>
       <c r="H23" s="61"/>
     </row>
     <row r="24" spans="2:8">
@@ -7974,7 +7974,7 @@
       </c>
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
-      <c r="G24" s="172"/>
+      <c r="G24" s="126"/>
       <c r="H24" s="61"/>
     </row>
     <row r="25" spans="2:8">
@@ -7987,7 +7987,7 @@
       </c>
       <c r="E25" s="38"/>
       <c r="F25" s="38"/>
-      <c r="G25" s="172"/>
+      <c r="G25" s="126"/>
       <c r="H25" s="61"/>
     </row>
     <row r="26" spans="2:8">
@@ -8000,7 +8000,7 @@
       </c>
       <c r="E26" s="38"/>
       <c r="F26" s="38"/>
-      <c r="G26" s="172"/>
+      <c r="G26" s="126"/>
       <c r="H26" s="61"/>
     </row>
     <row r="27" spans="2:8">
@@ -8009,7 +8009,7 @@
       <c r="D27" s="61"/>
       <c r="E27" s="38"/>
       <c r="F27" s="38"/>
-      <c r="G27" s="173"/>
+      <c r="G27" s="127"/>
       <c r="H27" s="61"/>
     </row>
     <row r="28" spans="2:8">
@@ -8018,7 +8018,7 @@
       <c r="D28" s="61"/>
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
-      <c r="G28" s="173"/>
+      <c r="G28" s="127"/>
       <c r="H28" s="61"/>
     </row>
     <row r="29" spans="2:8">
@@ -8027,7 +8027,7 @@
       <c r="D29" s="61"/>
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
-      <c r="G29" s="173"/>
+      <c r="G29" s="127"/>
       <c r="H29" s="61"/>
     </row>
   </sheetData>
@@ -8049,7 +8049,7 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A36" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
@@ -8076,12 +8076,12 @@
       <c r="C1" s="90"/>
       <c r="H1" s="91"/>
       <c r="I1" s="48"/>
-      <c r="J1" s="186"/>
+      <c r="J1" s="140"/>
     </row>
     <row r="2" spans="2:11">
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
     </row>
     <row r="3" spans="2:11" ht="29">
       <c r="B3" s="49" t="s">
@@ -8102,11 +8102,11 @@
       <c r="G3" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="H3" s="158" t="s">
+      <c r="H3" s="187" t="s">
         <v>184</v>
       </c>
-      <c r="I3" s="158"/>
-      <c r="J3" s="159"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="188"/>
       <c r="K3" s="52" t="s">
         <v>185</v>
       </c>
@@ -8124,7 +8124,7 @@
       <c r="G4" s="55"/>
       <c r="H4" s="54"/>
       <c r="I4" s="54"/>
-      <c r="J4" s="187"/>
+      <c r="J4" s="141"/>
       <c r="K4" s="56"/>
     </row>
     <row r="5" spans="2:11">
@@ -8144,15 +8144,15 @@
         <v>3</v>
       </c>
       <c r="G5" s="60"/>
-      <c r="H5" s="163" t="str">
+      <c r="H5" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#architectural-information"),
 "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
-      <c r="I5" s="175"/>
-      <c r="J5" s="175"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
       <c r="K5" s="62"/>
     </row>
     <row r="6" spans="2:11">
@@ -8172,21 +8172,21 @@
         <v>3</v>
       </c>
       <c r="G6" s="60"/>
-      <c r="H6" s="163" t="str">
+      <c r="H6" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),
 "Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
-      <c r="I6" s="174" t="str">
+      <c r="I6" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04h-Testing-Code-Quality.md#cross-site-scripting-flaws-mstg-arch-2-and-mstg-platform-2"),
 "Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
-      <c r="J6" s="168" t="str">
+      <c r="J6" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
@@ -8209,15 +8209,15 @@
         <v>3</v>
       </c>
       <c r="G7" s="60"/>
-      <c r="H7" s="163" t="str">
+      <c r="H7" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#architectural-information"),
 "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
-      <c r="I7" s="175"/>
-      <c r="J7" s="175"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
       <c r="K7" s="62"/>
     </row>
     <row r="8" spans="2:11">
@@ -8237,15 +8237,15 @@
         <v>3</v>
       </c>
       <c r="G8" s="60"/>
-      <c r="H8" s="163" t="str">
+      <c r="H8" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#identifying-sensitive-data"),
 "Identifying Sensitive Data")</f>
         <v>Identifying Sensitive Data</v>
       </c>
-      <c r="I8" s="175"/>
-      <c r="J8" s="175"/>
+      <c r="I8" s="129"/>
+      <c r="J8" s="129"/>
       <c r="K8" s="62"/>
     </row>
     <row r="9" spans="2:11">
@@ -8265,15 +8265,15 @@
       <c r="G9" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="163" t="str">
+      <c r="H9" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#environmental-information"),
 "Environmental Information")</f>
         <v>Environmental Information</v>
       </c>
-      <c r="I9" s="175"/>
-      <c r="J9" s="175"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="129"/>
       <c r="K9" s="62"/>
     </row>
     <row r="10" spans="2:11">
@@ -8293,15 +8293,15 @@
       <c r="G10" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="163" t="str">
+      <c r="H10" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#mapping-the-application"),
 "Mapping the Application")</f>
         <v>Mapping the Application</v>
       </c>
-      <c r="I10" s="175"/>
-      <c r="J10" s="175"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="129"/>
       <c r="K10" s="62"/>
     </row>
     <row r="11" spans="2:11">
@@ -8321,21 +8321,21 @@
       <c r="G11" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="163" t="str">
+      <c r="H11" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"),
 "Principles of Testing")</f>
         <v>Principles of Testing</v>
       </c>
-      <c r="I11" s="174" t="str">
+      <c r="I11" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#penetration-testing-aka-pentesting"),
 "Penetration Testing (a.k.a. Pentesting)")</f>
         <v>Penetration Testing (a.k.a. Pentesting)</v>
       </c>
-      <c r="J11" s="174"/>
+      <c r="J11" s="128"/>
       <c r="K11" s="62"/>
     </row>
     <row r="12" spans="2:11" ht="29">
@@ -8355,15 +8355,15 @@
       <c r="G12" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="163" t="str">
+      <c r="H12" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04g-Testing-Cryptography.md#cryptographic-policy"),
 "Cryptographic policy")</f>
         <v>Cryptographic policy</v>
       </c>
-      <c r="I12" s="175"/>
-      <c r="J12" s="175"/>
+      <c r="I12" s="129"/>
+      <c r="J12" s="129"/>
       <c r="K12" s="62"/>
     </row>
     <row r="13" spans="2:11">
@@ -8383,15 +8383,15 @@
       <c r="G13" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="163" t="str">
+      <c r="H13" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"),
 "Testing enforced updating (MSTG-ARCH-9)")</f>
         <v>Testing enforced updating (MSTG-ARCH-9)</v>
       </c>
-      <c r="I13" s="175"/>
-      <c r="J13" s="175"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="129"/>
       <c r="K13" s="62"/>
     </row>
     <row r="14" spans="2:11">
@@ -8411,15 +8411,15 @@
       <c r="G14" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="163" t="str">
+      <c r="H14" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#security-testing-and-the-sdlc"),
 "Security Testing and the SDLC")</f>
         <v>Security Testing and the SDLC</v>
       </c>
-      <c r="I14" s="175"/>
-      <c r="J14" s="175"/>
+      <c r="I14" s="129"/>
+      <c r="J14" s="129"/>
       <c r="K14" s="62"/>
     </row>
     <row r="15" spans="2:11">
@@ -8433,9 +8433,9 @@
       <c r="E15" s="67"/>
       <c r="F15" s="68"/>
       <c r="G15" s="67"/>
-      <c r="H15" s="165"/>
-      <c r="I15" s="176"/>
-      <c r="J15" s="176"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
       <c r="K15" s="69"/>
     </row>
     <row r="16" spans="2:11" ht="29">
@@ -8455,12 +8455,12 @@
         <v>3</v>
       </c>
       <c r="G16" s="60"/>
-      <c r="H16" s="168" t="str">
+      <c r="H16" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
-      <c r="I16" s="175"/>
-      <c r="J16" s="175"/>
+      <c r="I16" s="129"/>
+      <c r="J16" s="129"/>
       <c r="K16" s="62"/>
     </row>
     <row r="17" spans="2:12">
@@ -8476,12 +8476,12 @@
       <c r="E17" s="58"/>
       <c r="F17" s="59"/>
       <c r="G17" s="60"/>
-      <c r="H17" s="168" t="str">
+      <c r="H17" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
-      <c r="I17" s="175"/>
-      <c r="J17" s="175"/>
+      <c r="I17" s="129"/>
+      <c r="J17" s="129"/>
       <c r="K17" s="62"/>
     </row>
     <row r="18" spans="2:12">
@@ -8501,12 +8501,12 @@
         <v>3</v>
       </c>
       <c r="G18" s="60"/>
-      <c r="H18" s="168" t="str">
+      <c r="H18" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-logs-for-sensitive-data-mstg-storage-3"),"Checking Logs for Sensitive Data (MSTG-STORAGE-3)")</f>
         <v>Checking Logs for Sensitive Data (MSTG-STORAGE-3)</v>
       </c>
-      <c r="I18" s="175"/>
-      <c r="J18" s="175"/>
+      <c r="I18" s="129"/>
+      <c r="J18" s="129"/>
       <c r="K18" s="62"/>
     </row>
     <row r="19" spans="2:12">
@@ -8526,12 +8526,12 @@
         <v>3</v>
       </c>
       <c r="G19" s="60"/>
-      <c r="H19" s="168" t="str">
+      <c r="H19" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)")</f>
         <v>Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)</v>
       </c>
-      <c r="I19" s="175"/>
-      <c r="J19" s="175"/>
+      <c r="I19" s="129"/>
+      <c r="J19" s="129"/>
       <c r="K19" s="62"/>
     </row>
     <row r="20" spans="2:12">
@@ -8551,12 +8551,12 @@
         <v>3</v>
       </c>
       <c r="G20" s="60"/>
-      <c r="H20" s="168" t="str">
+      <c r="H20" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#finding-sensitive-data-in-the-keyboard-cache-mstg-storage-5"),"Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)")</f>
         <v>Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)</v>
       </c>
-      <c r="I20" s="175"/>
-      <c r="J20" s="175"/>
+      <c r="I20" s="129"/>
+      <c r="J20" s="129"/>
       <c r="K20" s="62"/>
     </row>
     <row r="21" spans="2:12">
@@ -8576,12 +8576,12 @@
         <v>3</v>
       </c>
       <c r="G21" s="60"/>
-      <c r="H21" s="167" t="str">
+      <c r="H21" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-exposed-via-ipc-mechanisms-mstg-storage-6"),"Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)")</f>
         <v>Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)</v>
       </c>
-      <c r="I21" s="175"/>
-      <c r="J21" s="175"/>
+      <c r="I21" s="129"/>
+      <c r="J21" s="129"/>
       <c r="K21" s="62"/>
     </row>
     <row r="22" spans="2:12">
@@ -8601,12 +8601,12 @@
         <v>3</v>
       </c>
       <c r="G22" s="60"/>
-      <c r="H22" s="168" t="str">
+      <c r="H22" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosed-through-the-user-interface-mstg-storage-7"),"Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)")</f>
         <v>Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)</v>
       </c>
-      <c r="I22" s="175"/>
-      <c r="J22" s="175"/>
+      <c r="I22" s="129"/>
+      <c r="J22" s="129"/>
       <c r="K22" s="62"/>
     </row>
     <row r="23" spans="2:12">
@@ -8626,12 +8626,12 @@
       <c r="G23" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H23" s="168" t="str">
+      <c r="H23" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Testing Backups for Sensitive Data (MSTG-STORAGE-8)")</f>
         <v>Testing Backups for Sensitive Data (MSTG-STORAGE-8)</v>
       </c>
-      <c r="I23" s="175"/>
-      <c r="J23" s="175"/>
+      <c r="I23" s="129"/>
+      <c r="J23" s="129"/>
       <c r="K23" s="62"/>
     </row>
     <row r="24" spans="2:12">
@@ -8651,12 +8651,12 @@
       <c r="G24" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="168" t="str">
+      <c r="H24" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-auto-generated-screenshots-for-sensitive-information-mstg-storage-9"),"Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)")</f>
         <v>Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)</v>
       </c>
-      <c r="I24" s="175"/>
-      <c r="J24" s="175"/>
+      <c r="I24" s="129"/>
+      <c r="J24" s="129"/>
       <c r="K24" s="62"/>
     </row>
     <row r="25" spans="2:12">
@@ -8676,12 +8676,12 @@
       <c r="G25" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H25" s="168" t="str">
+      <c r="H25" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-memory-for-sensitive-data-mstg-storage-10"),"Testing Memory for Sensitive Data (MSTG-STORAGE-10)")</f>
         <v>Testing Memory for Sensitive Data (MSTG-STORAGE-10)</v>
       </c>
-      <c r="I25" s="175"/>
-      <c r="J25" s="175"/>
+      <c r="I25" s="129"/>
+      <c r="J25" s="129"/>
       <c r="K25" s="62"/>
     </row>
     <row r="26" spans="2:12" ht="29">
@@ -8701,12 +8701,12 @@
       <c r="G26" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H26" s="168" t="str">
+      <c r="H26" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
-      <c r="I26" s="175"/>
-      <c r="J26" s="175"/>
+      <c r="I26" s="129"/>
+      <c r="J26" s="129"/>
       <c r="K26" s="62"/>
       <c r="L26" s="93"/>
     </row>
@@ -8727,12 +8727,12 @@
       <c r="G27" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H27" s="170" t="str">
+      <c r="H27" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04i-Testing-user-interaction.md#testing-user-education-mstg-storage-12"),"Testing User Education (MSTG-STORAGE-12)")</f>
         <v>Testing User Education (MSTG-STORAGE-12)</v>
       </c>
-      <c r="I27" s="175"/>
-      <c r="J27" s="175"/>
+      <c r="I27" s="129"/>
+      <c r="J27" s="129"/>
       <c r="K27" s="62"/>
       <c r="L27" s="46"/>
     </row>
@@ -8747,9 +8747,9 @@
       <c r="E28" s="67"/>
       <c r="F28" s="68"/>
       <c r="G28" s="67"/>
-      <c r="H28" s="165"/>
-      <c r="I28" s="176"/>
-      <c r="J28" s="176"/>
+      <c r="H28" s="119"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="130"/>
       <c r="K28" s="69"/>
     </row>
     <row r="29" spans="2:12">
@@ -8769,12 +8769,12 @@
         <v>3</v>
       </c>
       <c r="G29" s="60"/>
-      <c r="H29" s="168" t="str">
+      <c r="H29" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="I29" s="175"/>
-      <c r="J29" s="175"/>
+      <c r="I29" s="129"/>
+      <c r="J29" s="129"/>
       <c r="K29" s="62"/>
     </row>
     <row r="30" spans="2:12">
@@ -8794,12 +8794,12 @@
         <v>3</v>
       </c>
       <c r="G30" s="60"/>
-      <c r="H30" s="167" t="str">
+      <c r="H30" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="I30" s="175"/>
-      <c r="J30" s="175"/>
+      <c r="I30" s="129"/>
+      <c r="J30" s="129"/>
       <c r="K30" s="62"/>
     </row>
     <row r="31" spans="2:12" ht="29">
@@ -8819,12 +8819,12 @@
         <v>3</v>
       </c>
       <c r="G31" s="60"/>
-      <c r="H31" s="167" t="str">
+      <c r="H31" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="I31" s="175"/>
-      <c r="J31" s="175"/>
+      <c r="I31" s="129"/>
+      <c r="J31" s="129"/>
       <c r="K31" s="62"/>
     </row>
     <row r="32" spans="2:12">
@@ -8844,12 +8844,12 @@
         <v>3</v>
       </c>
       <c r="G32" s="60"/>
-      <c r="H32" s="168" t="str">
+      <c r="H32" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)")</f>
         <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)</v>
       </c>
-      <c r="I32" s="175"/>
-      <c r="J32" s="175"/>
+      <c r="I32" s="129"/>
+      <c r="J32" s="129"/>
       <c r="K32" s="62"/>
     </row>
     <row r="33" spans="2:13">
@@ -8869,12 +8869,12 @@
         <v>3</v>
       </c>
       <c r="G33" s="60"/>
-      <c r="H33" s="168" t="str">
+      <c r="H33" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="I33" s="175"/>
-      <c r="J33" s="175"/>
+      <c r="I33" s="129"/>
+      <c r="J33" s="129"/>
       <c r="K33" s="62"/>
     </row>
     <row r="34" spans="2:13">
@@ -8894,12 +8894,12 @@
         <v>3</v>
       </c>
       <c r="G34" s="60"/>
-      <c r="H34" s="168" t="str">
+      <c r="H34" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6")," Testing Random Number Generation (MSTG-CRYPTO-6)")</f>
         <v xml:space="preserve"> Testing Random Number Generation (MSTG-CRYPTO-6)</v>
       </c>
-      <c r="I34" s="175"/>
-      <c r="J34" s="175"/>
+      <c r="I34" s="129"/>
+      <c r="J34" s="129"/>
       <c r="K34" s="62"/>
     </row>
     <row r="35" spans="2:13">
@@ -8913,9 +8913,9 @@
       <c r="E35" s="67"/>
       <c r="F35" s="68"/>
       <c r="G35" s="67"/>
-      <c r="H35" s="165"/>
-      <c r="I35" s="176"/>
-      <c r="J35" s="176"/>
+      <c r="H35" s="119"/>
+      <c r="I35" s="130"/>
+      <c r="J35" s="130"/>
       <c r="K35" s="69"/>
     </row>
     <row r="36" spans="2:13" ht="29">
@@ -8935,15 +8935,15 @@
         <v>3</v>
       </c>
       <c r="G36" s="60"/>
-      <c r="H36" s="168" t="str">
+      <c r="H36" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
-      <c r="I36" s="168" t="str">
+      <c r="I36" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J36" s="168"/>
+      <c r="J36" s="122"/>
       <c r="K36" s="62"/>
     </row>
     <row r="37" spans="2:13" ht="29">
@@ -8963,12 +8963,12 @@
         <v>3</v>
       </c>
       <c r="G37" s="60"/>
-      <c r="H37" s="168" t="str">
+      <c r="H37" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Testing Stateful Session Management (MSTG-AUTH-2)")</f>
         <v>Testing Stateful Session Management (MSTG-AUTH-2)</v>
       </c>
-      <c r="I37" s="175"/>
-      <c r="J37" s="175"/>
+      <c r="I37" s="129"/>
+      <c r="J37" s="129"/>
       <c r="K37" s="62"/>
     </row>
     <row r="38" spans="2:13" ht="29">
@@ -8988,15 +8988,15 @@
         <v>3</v>
       </c>
       <c r="G38" s="60"/>
-      <c r="H38" s="168" t="str">
+      <c r="H38" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)")</f>
         <v>Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)</v>
       </c>
-      <c r="I38" s="168" t="str">
+      <c r="I38" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J38" s="168"/>
+      <c r="J38" s="122"/>
       <c r="K38" s="62"/>
     </row>
     <row r="39" spans="2:13">
@@ -9012,12 +9012,12 @@
       <c r="E39" s="58"/>
       <c r="F39" s="59"/>
       <c r="G39" s="60"/>
-      <c r="H39" s="168" t="str">
+      <c r="H39" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Testing User Logout (MSTG-AUTH-4)")</f>
         <v>Testing User Logout (MSTG-AUTH-4)</v>
       </c>
-      <c r="I39" s="175"/>
-      <c r="J39" s="175"/>
+      <c r="I39" s="129"/>
+      <c r="J39" s="129"/>
       <c r="K39" s="62"/>
       <c r="M39" s="73"/>
     </row>
@@ -9038,12 +9038,12 @@
         <v>3</v>
       </c>
       <c r="G40" s="60"/>
-      <c r="H40" s="168" t="str">
+      <c r="H40" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
-      <c r="I40" s="175"/>
-      <c r="J40" s="175"/>
+      <c r="I40" s="129"/>
+      <c r="J40" s="129"/>
       <c r="K40" s="62"/>
       <c r="M40" s="73"/>
     </row>
@@ -9064,15 +9064,15 @@
         <v>3</v>
       </c>
       <c r="G41" s="60"/>
-      <c r="H41" s="168" t="str">
+      <c r="H41" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
-      <c r="I41" s="168" t="str">
+      <c r="I41" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
         <v>Dynamic Testing (MSTG-AUTH-6)</v>
       </c>
-      <c r="J41" s="168"/>
+      <c r="J41" s="122"/>
       <c r="K41" s="62"/>
     </row>
     <row r="42" spans="2:13" ht="29">
@@ -9092,12 +9092,12 @@
         <v>3</v>
       </c>
       <c r="G42" s="60"/>
-      <c r="H42" s="168" t="str">
+      <c r="H42" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Testing Session Timeout (MSTG-AUTH-7)")</f>
         <v>Testing Session Timeout (MSTG-AUTH-7)</v>
       </c>
-      <c r="I42" s="177"/>
-      <c r="J42" s="177"/>
+      <c r="I42" s="131"/>
+      <c r="J42" s="131"/>
       <c r="K42" s="74"/>
     </row>
     <row r="43" spans="2:13" ht="29">
@@ -9117,12 +9117,12 @@
       <c r="G43" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H43" s="168" t="str">
+      <c r="H43" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
-      <c r="I43" s="168"/>
-      <c r="J43" s="168"/>
+      <c r="I43" s="122"/>
+      <c r="J43" s="122"/>
       <c r="K43" s="62"/>
     </row>
     <row r="44" spans="2:13" ht="29">
@@ -9142,12 +9142,12 @@
       <c r="G44" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H44" s="167" t="str">
+      <c r="H44" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
-      <c r="I44" s="175"/>
-      <c r="J44" s="175"/>
+      <c r="I44" s="129"/>
+      <c r="J44" s="129"/>
       <c r="K44" s="62"/>
     </row>
     <row r="45" spans="2:13">
@@ -9167,12 +9167,12 @@
       <c r="G45" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H45" s="167" t="str">
+      <c r="H45" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
-      <c r="I45" s="175"/>
-      <c r="J45" s="175"/>
+      <c r="I45" s="129"/>
+      <c r="J45" s="129"/>
       <c r="K45" s="62"/>
     </row>
     <row r="46" spans="2:13" ht="29">
@@ -9192,15 +9192,15 @@
       <c r="G46" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H46" s="170" t="str">
+      <c r="H46" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"),
 "Testing Login Activity and Device Blocking (MSTG-AUTH-11)")</f>
         <v>Testing Login Activity and Device Blocking (MSTG-AUTH-11)</v>
       </c>
-      <c r="I46" s="175"/>
-      <c r="J46" s="175"/>
+      <c r="I46" s="129"/>
+      <c r="J46" s="129"/>
       <c r="K46" s="62"/>
     </row>
     <row r="47" spans="2:13">
@@ -9214,9 +9214,9 @@
       <c r="E47" s="67"/>
       <c r="F47" s="68"/>
       <c r="G47" s="67"/>
-      <c r="H47" s="165"/>
-      <c r="I47" s="176"/>
-      <c r="J47" s="176"/>
+      <c r="H47" s="119"/>
+      <c r="I47" s="130"/>
+      <c r="J47" s="130"/>
       <c r="K47" s="69"/>
     </row>
     <row r="48" spans="2:13" ht="29">
@@ -9236,12 +9236,12 @@
         <v>3</v>
       </c>
       <c r="G48" s="60"/>
-      <c r="H48" s="167" t="str">
+      <c r="H48" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
-      <c r="I48" s="174"/>
-      <c r="J48" s="174"/>
+      <c r="I48" s="128"/>
+      <c r="J48" s="128"/>
       <c r="K48" s="75"/>
     </row>
     <row r="49" spans="2:11" ht="43.5">
@@ -9261,15 +9261,15 @@
         <v>3</v>
       </c>
       <c r="G49" s="60"/>
-      <c r="H49" s="167" t="str">
+      <c r="H49" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
-      <c r="I49" s="174" t="str">
+      <c r="I49" s="128" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#app-transport-security-mstg-network-2"),"App Transport Security (MSTG-NETWORK-2)")</f>
         <v>App Transport Security (MSTG-NETWORK-2)</v>
       </c>
-      <c r="J49" s="174"/>
+      <c r="J49" s="128"/>
       <c r="K49" s="75"/>
     </row>
     <row r="50" spans="2:11" ht="29">
@@ -9289,12 +9289,12 @@
         <v>3</v>
       </c>
       <c r="G50" s="60"/>
-      <c r="H50" s="168" t="str">
+      <c r="H50" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
-      <c r="I50" s="175"/>
-      <c r="J50" s="175"/>
+      <c r="I50" s="129"/>
+      <c r="J50" s="129"/>
       <c r="K50" s="75"/>
     </row>
     <row r="51" spans="2:11" ht="29">
@@ -9314,12 +9314,12 @@
       <c r="G51" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H51" s="168" t="str">
+      <c r="H51" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
-      <c r="I51" s="175"/>
-      <c r="J51" s="175"/>
+      <c r="I51" s="129"/>
+      <c r="J51" s="129"/>
       <c r="K51" s="62"/>
     </row>
     <row r="52" spans="2:11" ht="29">
@@ -9339,12 +9339,12 @@
       <c r="G52" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H52" s="167" t="str">
+      <c r="H52" s="121" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
         <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
       </c>
-      <c r="I52" s="175"/>
-      <c r="J52" s="175"/>
+      <c r="I52" s="129"/>
+      <c r="J52" s="129"/>
       <c r="K52" s="62"/>
     </row>
     <row r="53" spans="2:11">
@@ -9364,15 +9364,15 @@
       <c r="G53" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="H53" s="168" t="str">
+      <c r="H53" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),
 "Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
-      <c r="I53" s="175"/>
-      <c r="J53" s="175"/>
+      <c r="I53" s="129"/>
+      <c r="J53" s="129"/>
       <c r="K53" s="62"/>
     </row>
     <row r="54" spans="2:11">
@@ -9386,9 +9386,9 @@
       <c r="E54" s="67"/>
       <c r="F54" s="68"/>
       <c r="G54" s="67"/>
-      <c r="H54" s="165"/>
-      <c r="I54" s="176"/>
-      <c r="J54" s="176"/>
+      <c r="H54" s="119"/>
+      <c r="I54" s="130"/>
+      <c r="J54" s="130"/>
       <c r="K54" s="69"/>
     </row>
     <row r="55" spans="2:11">
@@ -9408,12 +9408,12 @@
         <v>3</v>
       </c>
       <c r="G55" s="60"/>
-      <c r="H55" s="168" t="str">
+      <c r="H55" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Testing App Permissions (MSTG-PLATFORM-1)")</f>
         <v>Testing App Permissions (MSTG-PLATFORM-1)</v>
       </c>
-      <c r="I55" s="175"/>
-      <c r="J55" s="175"/>
+      <c r="I55" s="129"/>
+      <c r="J55" s="129"/>
       <c r="K55" s="62"/>
     </row>
     <row r="56" spans="2:11" ht="29">
@@ -9433,12 +9433,12 @@
         <v>3</v>
       </c>
       <c r="G56" s="60"/>
-      <c r="H56" s="168" t="str">
+      <c r="H56" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),"Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
-      <c r="I56" s="175"/>
-      <c r="J56" s="175"/>
+      <c r="I56" s="129"/>
+      <c r="J56" s="129"/>
       <c r="K56" s="62"/>
     </row>
     <row r="57" spans="2:11" ht="29">
@@ -9458,12 +9458,12 @@
         <v>3</v>
       </c>
       <c r="G57" s="60"/>
-      <c r="H57" s="168" t="str">
+      <c r="H57" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Testing Custom URL Schemes (MSTG-PLATFORM-3)")</f>
         <v>Testing Custom URL Schemes (MSTG-PLATFORM-3)</v>
       </c>
-      <c r="I57" s="175"/>
-      <c r="J57" s="175"/>
+      <c r="I57" s="129"/>
+      <c r="J57" s="129"/>
       <c r="K57" s="62"/>
     </row>
     <row r="58" spans="2:11">
@@ -9483,15 +9483,15 @@
         <v>3</v>
       </c>
       <c r="G58" s="60"/>
-      <c r="H58" s="163" t="str">
+      <c r="H58" s="117" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"),
 "Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)")</f>
         <v>Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)</v>
       </c>
-      <c r="I58" s="175"/>
-      <c r="J58" s="175"/>
+      <c r="I58" s="129"/>
+      <c r="J58" s="129"/>
       <c r="K58" s="62"/>
     </row>
     <row r="59" spans="2:11">
@@ -9511,12 +9511,12 @@
         <v>3</v>
       </c>
       <c r="G59" s="60"/>
-      <c r="H59" s="168" t="str">
+      <c r="H59" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-ios-webviews-mstg-platform-5"),"Testing iOS WebViews (MSTG-PLATFORM-5)")</f>
         <v>Testing iOS WebViews (MSTG-PLATFORM-5)</v>
       </c>
-      <c r="I59" s="175"/>
-      <c r="J59" s="175"/>
+      <c r="I59" s="129"/>
+      <c r="J59" s="129"/>
       <c r="K59" s="62"/>
     </row>
     <row r="60" spans="2:11" ht="29">
@@ -9536,12 +9536,12 @@
         <v>3</v>
       </c>
       <c r="G60" s="60"/>
-      <c r="H60" s="168" t="str">
+      <c r="H60" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Testing WebView Protocol Handlers (MSTG-PLATFORM-6)")</f>
         <v>Testing WebView Protocol Handlers (MSTG-PLATFORM-6)</v>
       </c>
-      <c r="I60" s="175"/>
-      <c r="J60" s="175"/>
+      <c r="I60" s="129"/>
+      <c r="J60" s="129"/>
       <c r="K60" s="62"/>
     </row>
     <row r="61" spans="2:11" ht="29">
@@ -9561,12 +9561,12 @@
         <v>3</v>
       </c>
       <c r="G61" s="60"/>
-      <c r="H61" s="168" t="str">
+      <c r="H61" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#determining-whether-native-methods-are-exposed-through-webviews-mstg-platform-7"),"Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)")</f>
         <v>Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)</v>
       </c>
-      <c r="I61" s="175"/>
-      <c r="J61" s="175"/>
+      <c r="I61" s="129"/>
+      <c r="J61" s="129"/>
       <c r="K61" s="62"/>
     </row>
     <row r="62" spans="2:11" ht="29">
@@ -9586,12 +9586,12 @@
         <v>3</v>
       </c>
       <c r="G62" s="60"/>
-      <c r="H62" s="168" t="str">
+      <c r="H62" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Testing Object Persistence (MSTG-PLATFORM-8)")</f>
         <v>Testing Object Persistence (MSTG-PLATFORM-8)</v>
       </c>
-      <c r="I62" s="175"/>
-      <c r="J62" s="175"/>
+      <c r="I62" s="129"/>
+      <c r="J62" s="129"/>
       <c r="K62" s="62"/>
     </row>
     <row r="63" spans="2:11">
@@ -9605,9 +9605,9 @@
       <c r="E63" s="67"/>
       <c r="F63" s="68"/>
       <c r="G63" s="67"/>
-      <c r="H63" s="165"/>
-      <c r="I63" s="176"/>
-      <c r="J63" s="176"/>
+      <c r="H63" s="119"/>
+      <c r="I63" s="130"/>
+      <c r="J63" s="130"/>
       <c r="K63" s="69"/>
     </row>
     <row r="64" spans="2:11">
@@ -9627,12 +9627,12 @@
         <v>3</v>
       </c>
       <c r="G64" s="60"/>
-      <c r="H64" s="168" t="str">
+      <c r="H64" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Making Sure that the App Is Properly Signed (MSTG-CODE-1)")</f>
         <v>Making Sure that the App Is Properly Signed (MSTG-CODE-1)</v>
       </c>
-      <c r="I64" s="175"/>
-      <c r="J64" s="175"/>
+      <c r="I64" s="129"/>
+      <c r="J64" s="129"/>
       <c r="K64" s="62"/>
     </row>
     <row r="65" spans="2:11">
@@ -9652,12 +9652,12 @@
         <v>3</v>
       </c>
       <c r="G65" s="60"/>
-      <c r="H65" s="168" t="str">
+      <c r="H65" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#determining-whether-the-app-is-debuggable-mstg-code-2"),"Determining Whether the App is Debuggable (MSTG-CODE-2)")</f>
         <v>Determining Whether the App is Debuggable (MSTG-CODE-2)</v>
       </c>
-      <c r="I65" s="175"/>
-      <c r="J65" s="175"/>
+      <c r="I65" s="129"/>
+      <c r="J65" s="129"/>
       <c r="K65" s="62"/>
     </row>
     <row r="66" spans="2:11">
@@ -9677,12 +9677,12 @@
         <v>3</v>
       </c>
       <c r="G66" s="60"/>
-      <c r="H66" s="168" t="str">
+      <c r="H66" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-symbols-mstg-code-3"),"Finding Debugging Symbols (MSTG-CODE-3)")</f>
         <v>Finding Debugging Symbols (MSTG-CODE-3)</v>
       </c>
-      <c r="I66" s="175"/>
-      <c r="J66" s="175"/>
+      <c r="I66" s="129"/>
+      <c r="J66" s="129"/>
       <c r="K66" s="62"/>
     </row>
     <row r="67" spans="2:11">
@@ -9702,12 +9702,12 @@
         <v>3</v>
       </c>
       <c r="G67" s="60"/>
-      <c r="H67" s="168" t="str">
+      <c r="H67" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-code-and-verbose-error-logging-mstg-code-4"),"Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)")</f>
         <v>Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)</v>
       </c>
-      <c r="I67" s="175"/>
-      <c r="J67" s="175"/>
+      <c r="I67" s="129"/>
+      <c r="J67" s="129"/>
       <c r="K67" s="62"/>
     </row>
     <row r="68" spans="2:11" ht="29">
@@ -9727,12 +9727,12 @@
         <v>3</v>
       </c>
       <c r="G68" s="60"/>
-      <c r="H68" s="170" t="str">
+      <c r="H68" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
-      <c r="I68" s="175"/>
-      <c r="J68" s="175"/>
+      <c r="I68" s="129"/>
+      <c r="J68" s="129"/>
       <c r="K68" s="62"/>
     </row>
     <row r="69" spans="2:11">
@@ -9752,12 +9752,12 @@
         <v>3</v>
       </c>
       <c r="G69" s="60"/>
-      <c r="H69" s="168" t="str">
+      <c r="H69" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
-      <c r="I69" s="175"/>
-      <c r="J69" s="175"/>
+      <c r="I69" s="129"/>
+      <c r="J69" s="129"/>
       <c r="K69" s="62"/>
     </row>
     <row r="70" spans="2:11">
@@ -9777,12 +9777,12 @@
         <v>3</v>
       </c>
       <c r="G70" s="60"/>
-      <c r="H70" s="168" t="str">
+      <c r="H70" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
-      <c r="I70" s="175"/>
-      <c r="J70" s="175"/>
+      <c r="I70" s="129"/>
+      <c r="J70" s="129"/>
       <c r="K70" s="62"/>
     </row>
     <row r="71" spans="2:11">
@@ -9802,12 +9802,12 @@
         <v>3</v>
       </c>
       <c r="G71" s="60"/>
-      <c r="H71" s="168" t="str">
+      <c r="H71" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#memory-corruption-bugs-mstg-code-8"),"Memory Corruption Bugs (MSTG-CODE-8)")</f>
         <v>Memory Corruption Bugs (MSTG-CODE-8)</v>
       </c>
-      <c r="I71" s="175"/>
-      <c r="J71" s="175"/>
+      <c r="I71" s="129"/>
+      <c r="J71" s="129"/>
       <c r="K71" s="62"/>
     </row>
     <row r="72" spans="2:11" ht="29">
@@ -9827,12 +9827,12 @@
         <v>3</v>
       </c>
       <c r="G72" s="60"/>
-      <c r="H72" s="168" t="str">
+      <c r="H72" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Make Sure That Free Security Features Are Activated (MSTG-CODE-9)")</f>
         <v>Make Sure That Free Security Features Are Activated (MSTG-CODE-9)</v>
       </c>
-      <c r="I72" s="175"/>
-      <c r="J72" s="175"/>
+      <c r="I72" s="129"/>
+      <c r="J72" s="129"/>
       <c r="K72" s="62"/>
     </row>
     <row r="73" spans="2:11">
@@ -9842,9 +9842,9 @@
       <c r="E73" s="80"/>
       <c r="F73" s="80"/>
       <c r="G73" s="80"/>
-      <c r="H73" s="171"/>
-      <c r="I73" s="178"/>
-      <c r="J73" s="178"/>
+      <c r="H73" s="125"/>
+      <c r="I73" s="132"/>
+      <c r="J73" s="132"/>
       <c r="K73" s="94"/>
     </row>
     <row r="74" spans="2:11">
@@ -9854,9 +9854,9 @@
       <c r="E74" s="28"/>
       <c r="F74" s="28"/>
       <c r="G74" s="28"/>
-      <c r="H74" s="172"/>
-      <c r="I74" s="172"/>
-      <c r="J74" s="172"/>
+      <c r="H74" s="126"/>
+      <c r="I74" s="126"/>
+      <c r="J74" s="126"/>
       <c r="K74" s="96"/>
     </row>
     <row r="75" spans="2:11">
@@ -9866,9 +9866,9 @@
       <c r="E75" s="28"/>
       <c r="F75" s="28"/>
       <c r="G75" s="28"/>
-      <c r="H75" s="172"/>
-      <c r="I75" s="172"/>
-      <c r="J75" s="172"/>
+      <c r="H75" s="126"/>
+      <c r="I75" s="126"/>
+      <c r="J75" s="126"/>
       <c r="K75" s="96"/>
     </row>
     <row r="76" spans="2:11">
@@ -9878,9 +9878,9 @@
       <c r="E76" s="28"/>
       <c r="F76" s="28"/>
       <c r="G76" s="28"/>
-      <c r="H76" s="172"/>
-      <c r="I76" s="172"/>
-      <c r="J76" s="172"/>
+      <c r="H76" s="126"/>
+      <c r="I76" s="126"/>
+      <c r="J76" s="126"/>
       <c r="K76" s="96"/>
     </row>
     <row r="77" spans="2:11">
@@ -9892,9 +9892,9 @@
       <c r="E77" s="28"/>
       <c r="F77" s="28"/>
       <c r="G77" s="28"/>
-      <c r="H77" s="172"/>
-      <c r="I77" s="172"/>
-      <c r="J77" s="172"/>
+      <c r="H77" s="126"/>
+      <c r="I77" s="126"/>
+      <c r="J77" s="126"/>
       <c r="K77" s="96"/>
     </row>
     <row r="78" spans="2:11" ht="29">
@@ -9908,9 +9908,9 @@
       <c r="E78" s="28"/>
       <c r="F78" s="28"/>
       <c r="G78" s="28"/>
-      <c r="H78" s="172"/>
-      <c r="I78" s="172"/>
-      <c r="J78" s="172"/>
+      <c r="H78" s="126"/>
+      <c r="I78" s="126"/>
+      <c r="J78" s="126"/>
       <c r="K78" s="96"/>
     </row>
     <row r="79" spans="2:11">
@@ -9924,9 +9924,9 @@
       <c r="E79" s="28"/>
       <c r="F79" s="28"/>
       <c r="G79" s="28"/>
-      <c r="H79" s="172"/>
-      <c r="I79" s="172"/>
-      <c r="J79" s="172"/>
+      <c r="H79" s="126"/>
+      <c r="I79" s="126"/>
+      <c r="J79" s="126"/>
       <c r="K79" s="96"/>
     </row>
     <row r="80" spans="2:11">
@@ -9940,9 +9940,9 @@
       <c r="E80" s="28"/>
       <c r="F80" s="28"/>
       <c r="G80" s="28"/>
-      <c r="H80" s="172"/>
-      <c r="I80" s="172"/>
-      <c r="J80" s="172"/>
+      <c r="H80" s="126"/>
+      <c r="I80" s="126"/>
+      <c r="J80" s="126"/>
       <c r="K80" s="96"/>
     </row>
     <row r="81" spans="2:11">
@@ -9956,9 +9956,9 @@
       <c r="E81" s="28"/>
       <c r="F81" s="28"/>
       <c r="G81" s="28"/>
-      <c r="H81" s="172"/>
-      <c r="I81" s="172"/>
-      <c r="J81" s="172"/>
+      <c r="H81" s="126"/>
+      <c r="I81" s="126"/>
+      <c r="J81" s="126"/>
       <c r="K81" s="96"/>
     </row>
     <row r="82" spans="2:11">
@@ -9968,9 +9968,9 @@
       <c r="E82" s="28"/>
       <c r="F82" s="28"/>
       <c r="G82" s="28"/>
-      <c r="H82" s="172"/>
-      <c r="I82" s="173"/>
-      <c r="J82" s="173"/>
+      <c r="H82" s="126"/>
+      <c r="I82" s="127"/>
+      <c r="J82" s="127"/>
       <c r="K82" s="96"/>
     </row>
     <row r="83" spans="2:11">
@@ -9980,9 +9980,9 @@
       <c r="E83" s="28"/>
       <c r="F83" s="28"/>
       <c r="G83" s="28"/>
-      <c r="H83" s="172"/>
-      <c r="I83" s="173"/>
-      <c r="J83" s="173"/>
+      <c r="H83" s="126"/>
+      <c r="I83" s="127"/>
+      <c r="J83" s="127"/>
       <c r="K83" s="96"/>
     </row>
     <row r="84" spans="2:11">
@@ -9992,9 +9992,9 @@
       <c r="E84" s="28"/>
       <c r="F84" s="28"/>
       <c r="G84" s="28"/>
-      <c r="H84" s="172"/>
-      <c r="I84" s="173"/>
-      <c r="J84" s="173"/>
+      <c r="H84" s="126"/>
+      <c r="I84" s="127"/>
+      <c r="J84" s="127"/>
       <c r="K84" s="96"/>
     </row>
     <row r="85" spans="2:11">
@@ -10004,9 +10004,9 @@
       <c r="E85" s="28"/>
       <c r="F85" s="28"/>
       <c r="G85" s="28"/>
-      <c r="H85" s="173"/>
-      <c r="I85" s="173"/>
-      <c r="J85" s="173"/>
+      <c r="H85" s="127"/>
+      <c r="I85" s="127"/>
+      <c r="J85" s="127"/>
       <c r="K85" s="96"/>
     </row>
   </sheetData>
@@ -10069,11 +10069,11 @@
         <v>206</v>
       </c>
       <c r="C1" s="90"/>
-      <c r="G1" s="173"/>
+      <c r="G1" s="127"/>
       <c r="H1" s="96"/>
     </row>
     <row r="2" spans="2:8">
-      <c r="G2" s="173"/>
+      <c r="G2" s="127"/>
       <c r="H2" s="96"/>
     </row>
     <row r="3" spans="2:8">
@@ -10092,7 +10092,7 @@
       <c r="F3" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="G3" s="179" t="s">
+      <c r="G3" s="133" t="s">
         <v>383</v>
       </c>
       <c r="H3" s="52" t="s">
@@ -10109,7 +10109,7 @@
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="67"/>
-      <c r="G4" s="180"/>
+      <c r="G4" s="134"/>
       <c r="H4" s="69"/>
     </row>
     <row r="5" spans="2:8" ht="29">
@@ -10128,7 +10128,7 @@
       <c r="F5" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="168" t="str">
+      <c r="G5" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#jailbreak-detection-mstg-resilience-1"),"Jailbreak Detection (MSTG-RESILIENCE-1)")</f>
         <v>Jailbreak Detection (MSTG-RESILIENCE-1)</v>
       </c>
@@ -10150,7 +10150,7 @@
       <c r="F6" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="181" t="str">
+      <c r="G6" s="135" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#anti-debugging-checks-mstg-resilience-2"),"Anti-Debugging Checks (MSTG-RESILIENCE-2)")</f>
         <v>Anti-Debugging Checks (MSTG-RESILIENCE-2)</v>
       </c>
@@ -10172,7 +10172,7 @@
       <c r="F7" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="181" t="str">
+      <c r="G7" s="135" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -10194,7 +10194,7 @@
       <c r="F8" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="188" t="s">
+      <c r="G8" s="142" t="s">
         <v>79</v>
       </c>
       <c r="H8" s="62"/>
@@ -10215,7 +10215,7 @@
       <c r="F9" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="189" t="s">
+      <c r="G9" s="143" t="s">
         <v>79</v>
       </c>
       <c r="H9" s="62"/>
@@ -10236,7 +10236,7 @@
       <c r="F10" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="188" t="s">
+      <c r="G10" s="142" t="s">
         <v>79</v>
       </c>
       <c r="H10" s="62"/>
@@ -10257,7 +10257,7 @@
       <c r="F11" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="184" t="s">
+      <c r="G11" s="138" t="s">
         <v>79</v>
       </c>
       <c r="H11" s="62"/>
@@ -10278,7 +10278,7 @@
       <c r="F12" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="184" t="s">
+      <c r="G12" s="138" t="s">
         <v>79</v>
       </c>
       <c r="H12" s="62"/>
@@ -10299,7 +10299,7 @@
       <c r="F13" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="189" t="s">
+      <c r="G13" s="143" t="s">
         <v>79</v>
       </c>
       <c r="H13" s="62"/>
@@ -10312,7 +10312,7 @@
       </c>
       <c r="E14" s="67"/>
       <c r="F14" s="67"/>
-      <c r="G14" s="180"/>
+      <c r="G14" s="134"/>
       <c r="H14" s="69"/>
     </row>
     <row r="15" spans="2:8" ht="29">
@@ -10331,7 +10331,7 @@
       <c r="F15" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="168" t="str">
+      <c r="G15" s="122" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#device-binding-mstg-resilience-10"),"Device Binding (MSTG-RESILIENCE-10)")</f>
         <v>Device Binding (MSTG-RESILIENCE-10)</v>
       </c>
@@ -10345,7 +10345,7 @@
       </c>
       <c r="E16" s="67"/>
       <c r="F16" s="67"/>
-      <c r="G16" s="180"/>
+      <c r="G16" s="134"/>
       <c r="H16" s="69"/>
     </row>
     <row r="17" spans="2:8" ht="43.5">
@@ -10364,7 +10364,7 @@
       <c r="F17" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="190" t="str">
+      <c r="G17" s="144" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -10386,7 +10386,7 @@
       <c r="F18" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="184" t="s">
+      <c r="G18" s="138" t="s">
         <v>79</v>
       </c>
       <c r="H18" s="62"/>
@@ -10397,7 +10397,7 @@
       <c r="D19" s="79"/>
       <c r="E19" s="80"/>
       <c r="F19" s="80"/>
-      <c r="G19" s="185"/>
+      <c r="G19" s="139"/>
       <c r="H19" s="81"/>
     </row>
     <row r="20" spans="2:8">
@@ -10406,7 +10406,7 @@
       <c r="D20" s="96"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="172"/>
+      <c r="G20" s="126"/>
       <c r="H20" s="96"/>
     </row>
     <row r="21" spans="2:8">
@@ -10415,7 +10415,7 @@
       <c r="D21" s="96"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
-      <c r="G21" s="172"/>
+      <c r="G21" s="126"/>
       <c r="H21" s="96"/>
     </row>
     <row r="22" spans="2:8">
@@ -10426,7 +10426,7 @@
       <c r="D22" s="96"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
-      <c r="G22" s="172"/>
+      <c r="G22" s="126"/>
       <c r="H22" s="96"/>
     </row>
     <row r="23" spans="2:8" ht="29">
@@ -10439,7 +10439,7 @@
       </c>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
-      <c r="G23" s="172"/>
+      <c r="G23" s="126"/>
       <c r="H23" s="96"/>
     </row>
     <row r="24" spans="2:8">
@@ -10452,7 +10452,7 @@
       </c>
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
-      <c r="G24" s="172"/>
+      <c r="G24" s="126"/>
       <c r="H24" s="96"/>
     </row>
     <row r="25" spans="2:8">
@@ -10465,7 +10465,7 @@
       </c>
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
-      <c r="G25" s="172"/>
+      <c r="G25" s="126"/>
       <c r="H25" s="96"/>
     </row>
     <row r="26" spans="2:8">
@@ -10478,7 +10478,7 @@
       </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
-      <c r="G26" s="172"/>
+      <c r="G26" s="126"/>
       <c r="H26" s="96"/>
     </row>
     <row r="27" spans="2:8">
@@ -10487,7 +10487,7 @@
       <c r="D27" s="96"/>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
-      <c r="G27" s="173"/>
+      <c r="G27" s="127"/>
       <c r="H27" s="96"/>
     </row>
     <row r="28" spans="2:8">
@@ -10496,7 +10496,7 @@
       <c r="D28" s="96"/>
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
-      <c r="G28" s="173"/>
+      <c r="G28" s="127"/>
       <c r="H28" s="96"/>
     </row>
     <row r="29" spans="2:8">
@@ -10505,7 +10505,7 @@
       <c r="D29" s="96"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
-      <c r="G29" s="173"/>
+      <c r="G29" s="127"/>
       <c r="H29" s="96"/>
     </row>
     <row r="30" spans="2:8">
@@ -10589,7 +10589,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E25" activeCellId="29" sqref="A20 B20 C20 D20 E20 A21 B21 C21 D21 E21 A22 B22 C22 D22 E22 A23 B23 C23 D23 E23 A24 B24 C24 D24 E24 A25 B25 C25 D25 E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.9140625" defaultRowHeight="15.5"/>
@@ -10600,10 +10600,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="189" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="160"/>
+      <c r="B1" s="189"/>
       <c r="C1" s="10"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -11007,10 +11007,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.08203125" defaultRowHeight="15.5"/>
@@ -11022,10 +11022,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="190" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="161"/>
+      <c r="B1" s="190"/>
       <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:5">
@@ -11128,6 +11128,108 @@
       </c>
       <c r="E7" s="100" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="108.5">
+      <c r="A8" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="14">
+        <v>43641</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" s="105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="14">
+        <v>43642</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="46.5">
+      <c r="A10" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="14">
+        <v>43649</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D11" s="14">
+        <v>43672</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" s="14">
+        <v>43674</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="46.5">
+      <c r="A13" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="113" t="s">
+        <v>380</v>
+      </c>
+      <c r="C13" s="105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D13" s="114">
+        <v>43685</v>
+      </c>
+      <c r="E13" s="115" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>